<commit_message>
fix: update overtime template Excel file
</commit_message>
<xml_diff>
--- a/src/assets/overtime_template.xlsx
+++ b/src/assets/overtime_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\magda.dubiel\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bbcgroup365.sharepoint.com/sites/CEP-O-OgolnePL-HR/Shared Documents/HR/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4853A9B9-1D28-4D7F-B792-A1A904D0EE10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="27" documentId="13_ncr:1_{4853A9B9-1D28-4D7F-B792-A1A904D0EE10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EDDCF0AE-9EEC-4C5F-81C2-C0732B928168}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5C54F8F0-E29B-4B1D-B5B0-84E7A0453ECD}"/>
+    <workbookView xWindow="-90" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{5C54F8F0-E29B-4B1D-B5B0-84E7A0453ECD}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="78">
   <si>
     <t>MIESIĘCZNA 
 KARTA EWIDENCJI CZASU PRACY</t>
@@ -400,6 +400,10 @@
   <si>
     <t>UM</t>
   </si>
+  <si>
+    <t>żółte wiersze do uzupełnienia obowiązkowo
+pozostałe opcjonalnie</t>
+  </si>
 </sst>
 </file>
 
@@ -408,7 +412,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="h:mm;@"/>
   </numFmts>
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -583,8 +587,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -618,6 +630,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -785,7 +803,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -853,9 +871,6 @@
     <xf numFmtId="0" fontId="13" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="4" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -883,157 +898,170 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="23" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1043,9 +1071,47 @@
   <dxfs count="134">
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
         <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCDCD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFE1E1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
       </font>
       <fill>
         <patternFill patternType="none">
@@ -1055,9 +1121,7 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color rgb="FF005C00"/>
+        <color rgb="FFC00000"/>
       </font>
       <fill>
         <patternFill patternType="none">
@@ -1079,7 +1143,9 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FFC00000"/>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FF005C00"/>
       </font>
       <fill>
         <patternFill patternType="none">
@@ -1101,7 +1167,9 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FFC00000"/>
+        <b val="0"/>
+        <i val="0"/>
+        <color auto="1"/>
       </font>
       <fill>
         <patternFill patternType="none">
@@ -1115,65 +1183,43 @@
       </font>
       <fill>
         <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCDCD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFFE1E1"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCDCD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color rgb="FF005C00"/>
+        <color rgb="FFC00000"/>
       </font>
       <fill>
         <patternFill patternType="none">
@@ -1183,9 +1229,7 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color rgb="FF005C00"/>
+        <color rgb="FFC00000"/>
       </font>
       <fill>
         <patternFill patternType="none">
@@ -1194,29 +1238,10 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCDEBFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF5F9FD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color auto="1"/>
+        <color rgb="FF005C00"/>
       </font>
       <fill>
         <patternFill patternType="none">
@@ -1238,7 +1263,9 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FFC00000"/>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FF005C00"/>
       </font>
       <fill>
         <patternFill patternType="none">
@@ -1248,7 +1275,9 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FFC00000"/>
+        <b val="0"/>
+        <i val="0"/>
+        <color auto="1"/>
       </font>
       <fill>
         <patternFill patternType="none">
@@ -1258,218 +1287,206 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
         <color auto="1"/>
       </font>
       <fill>
         <patternFill>
+          <bgColor rgb="FFF5F9FD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCDEBFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF006600"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF006600"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF0000FF"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF0000FF"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF0000FF"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF0000FF"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF0000FF"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF0000FF"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCDCD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFFE1E1"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCDCD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF006600"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF006600"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF0000FF"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF0000FF"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF0000FF"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FFC00000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF0000FF"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF0000FF"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF0000FF"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCDCD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCDEBFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF5F9FD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color auto="1"/>
       </font>
       <fill>
         <patternFill patternType="none">
@@ -1479,9 +1496,7 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color rgb="FF005C00"/>
+        <color rgb="FFC00000"/>
       </font>
       <fill>
         <patternFill patternType="none">
@@ -1515,7 +1530,9 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FFC00000"/>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FF005C00"/>
       </font>
       <fill>
         <patternFill patternType="none">
@@ -1525,7 +1542,9 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FFC00000"/>
+        <b val="0"/>
+        <i val="0"/>
+        <color auto="1"/>
       </font>
       <fill>
         <patternFill patternType="none">
@@ -1535,77 +1554,105 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
         <color auto="1"/>
       </font>
       <fill>
         <patternFill>
+          <bgColor rgb="FFF5F9FD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCDEBFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF008000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF008000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF0000FF"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF5F9FD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCDEBFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCDCD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFFE1E1"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF008000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF008000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF0000FF"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF5F9FD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCDEBFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCDEBFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF5F9FD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color auto="1"/>
+        <color rgb="FFC00000"/>
       </font>
       <fill>
         <patternFill patternType="none">
@@ -1615,9 +1662,7 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color rgb="FF005C00"/>
+        <color rgb="FFC00000"/>
       </font>
       <fill>
         <patternFill patternType="none">
@@ -1627,7 +1672,9 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FFC00000"/>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FF005C00"/>
       </font>
       <fill>
         <patternFill patternType="none">
@@ -1637,26 +1684,6 @@
     </dxf>
     <dxf>
       <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <color rgb="FF005C00"/>
@@ -1669,7 +1696,9 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FFC00000"/>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FF005C00"/>
       </font>
       <fill>
         <patternFill patternType="none">
@@ -1679,29 +1708,9 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
         <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE1E1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCDCD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color rgb="FF005C00"/>
       </font>
       <fill>
         <patternFill patternType="none">
@@ -1711,41 +1720,60 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
         <color auto="1"/>
       </font>
       <fill>
         <patternFill>
+          <bgColor rgb="FFF5F9FD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCDEBFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCDCD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFFE1E1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCDCD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1837,12 +1865,43 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
         <color rgb="FFFF0000"/>
       </font>
     </dxf>
     <dxf>
       <font>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FFFF0000"/>
       </font>
     </dxf>
@@ -1863,20 +1922,98 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF0000FF"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF0000FF"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF0000FF"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF0000FF"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF0000FF"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF0000FF"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FFC00000"/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
         <b/>
         <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
+        <color rgb="FF006600"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF006600"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFE5E5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD3E6F5"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -1884,96 +2021,44 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FF006600"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FF006600"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
         <color rgb="FFC00000"/>
       </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF0000FF"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF0000FF"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF0000FF"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF0000FF"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF0000FF"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF0000FF"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF006600"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF006600"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE5E5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
       <fill>
         <patternFill>
           <bgColor theme="4" tint="0.59996337778862885"/>
@@ -1981,18 +2066,46 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD3E6F5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
         <color auto="1"/>
       </font>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFFD9D9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFE7E7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
           <bgColor theme="9" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
@@ -2001,14 +2114,19 @@
       <font>
         <b val="0"/>
         <i val="0"/>
-        <color rgb="FF006600"/>
+        <color rgb="FF005000"/>
       </font>
     </dxf>
     <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
-        <color rgb="FF006600"/>
+        <color rgb="FF005000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
       </font>
     </dxf>
     <dxf>
@@ -2020,109 +2138,47 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCDCD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFE1E1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFD9D9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE7E7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color rgb="FF005000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color rgb="FF005000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color rgb="FF005C00"/>
       </font>
       <fill>
         <patternFill patternType="none">
@@ -2142,7 +2198,9 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FFC00000"/>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FF005C00"/>
       </font>
       <fill>
         <patternFill patternType="none">
@@ -2152,39 +2210,9 @@
     </dxf>
     <dxf>
       <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE1E1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCDCD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
-        <color auto="1"/>
+        <color rgb="FF005C00"/>
       </font>
       <fill>
         <patternFill patternType="none">
@@ -2208,7 +2236,7 @@
       <font>
         <b val="0"/>
         <i val="0"/>
-        <color rgb="FF005C00"/>
+        <color auto="1"/>
       </font>
       <fill>
         <patternFill patternType="none">
@@ -2546,295 +2574,297 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14D71DC9-2596-441F-B45A-63A457CE14D1}">
-  <dimension ref="A1:AI27"/>
+  <dimension ref="A1:AI29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Y27" sqref="Y27:AA27"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="19.140625" customWidth="1"/>
-    <col min="3" max="3" width="17.7109375" customWidth="1"/>
+    <col min="2" max="2" width="19.109375" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="74" t="s">
+    <row r="1" spans="1:35" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="75"/>
-      <c r="C1" s="75"/>
-      <c r="D1" s="75"/>
-      <c r="E1" s="75"/>
-      <c r="F1" s="75"/>
-      <c r="G1" s="75"/>
-      <c r="H1" s="76"/>
-      <c r="I1" s="73" t="s">
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="73"/>
-      <c r="K1" s="73"/>
-      <c r="L1" s="73"/>
-      <c r="M1" s="73"/>
-      <c r="N1" s="73"/>
-      <c r="O1" s="72"/>
-      <c r="P1" s="72"/>
-      <c r="Q1" s="72"/>
-      <c r="R1" s="72"/>
-      <c r="S1" s="72"/>
-      <c r="T1" s="72"/>
-      <c r="U1" s="72"/>
-      <c r="V1" s="72"/>
-      <c r="W1" s="72"/>
-      <c r="X1" s="72"/>
-      <c r="Y1" s="72"/>
-      <c r="Z1" s="72"/>
-      <c r="AA1" s="80" t="s">
+      <c r="J1" s="38"/>
+      <c r="K1" s="38"/>
+      <c r="L1" s="38"/>
+      <c r="M1" s="38"/>
+      <c r="N1" s="38"/>
+      <c r="O1" s="39"/>
+      <c r="P1" s="39"/>
+      <c r="Q1" s="39"/>
+      <c r="R1" s="39"/>
+      <c r="S1" s="39"/>
+      <c r="T1" s="39"/>
+      <c r="U1" s="39"/>
+      <c r="V1" s="39"/>
+      <c r="W1" s="39"/>
+      <c r="X1" s="39"/>
+      <c r="Y1" s="39"/>
+      <c r="Z1" s="39"/>
+      <c r="AA1" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="AB1" s="80"/>
-      <c r="AC1" s="80"/>
-      <c r="AD1" s="80"/>
-      <c r="AE1" s="80"/>
-      <c r="AF1" s="80"/>
-      <c r="AG1" s="80"/>
-      <c r="AH1" s="80"/>
-      <c r="AI1" s="80"/>
+      <c r="AB1" s="40"/>
+      <c r="AC1" s="40"/>
+      <c r="AD1" s="40"/>
+      <c r="AE1" s="40"/>
+      <c r="AF1" s="40"/>
+      <c r="AG1" s="40"/>
+      <c r="AH1" s="40"/>
+      <c r="AI1" s="40"/>
     </row>
-    <row r="2" spans="1:35" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="77"/>
-      <c r="B2" s="78"/>
-      <c r="C2" s="78"/>
-      <c r="D2" s="78"/>
-      <c r="E2" s="78"/>
-      <c r="F2" s="78"/>
-      <c r="G2" s="78"/>
-      <c r="H2" s="79"/>
-      <c r="I2" s="73" t="s">
+    <row r="2" spans="1:35" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="35"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="73"/>
-      <c r="K2" s="73"/>
-      <c r="L2" s="73"/>
-      <c r="M2" s="73"/>
-      <c r="N2" s="73"/>
-      <c r="O2" s="70"/>
-      <c r="P2" s="70"/>
-      <c r="Q2" s="70"/>
-      <c r="R2" s="70"/>
-      <c r="S2" s="70"/>
-      <c r="T2" s="70"/>
-      <c r="U2" s="70"/>
-      <c r="V2" s="70"/>
+      <c r="J2" s="38"/>
+      <c r="K2" s="38"/>
+      <c r="L2" s="38"/>
+      <c r="M2" s="38"/>
+      <c r="N2" s="38"/>
+      <c r="O2" s="41"/>
+      <c r="P2" s="41"/>
+      <c r="Q2" s="41"/>
+      <c r="R2" s="41"/>
+      <c r="S2" s="41"/>
+      <c r="T2" s="41"/>
+      <c r="U2" s="41"/>
+      <c r="V2" s="41"/>
       <c r="W2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="X2" s="81"/>
-      <c r="Y2" s="82"/>
-      <c r="Z2" s="82"/>
-      <c r="AA2" s="80"/>
-      <c r="AB2" s="80"/>
-      <c r="AC2" s="80"/>
-      <c r="AD2" s="80"/>
-      <c r="AE2" s="80"/>
-      <c r="AF2" s="80"/>
-      <c r="AG2" s="80"/>
-      <c r="AH2" s="80"/>
-      <c r="AI2" s="80"/>
+      <c r="X2" s="42"/>
+      <c r="Y2" s="43"/>
+      <c r="Z2" s="43"/>
+      <c r="AA2" s="40"/>
+      <c r="AB2" s="40"/>
+      <c r="AC2" s="40"/>
+      <c r="AD2" s="40"/>
+      <c r="AE2" s="40"/>
+      <c r="AF2" s="40"/>
+      <c r="AG2" s="40"/>
+      <c r="AH2" s="40"/>
+      <c r="AI2" s="40"/>
     </row>
-    <row r="3" spans="1:35" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="71" t="s">
+    <row r="3" spans="1:35" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="71"/>
-      <c r="C3" s="83"/>
-      <c r="D3" s="83"/>
-      <c r="E3" s="83"/>
-      <c r="F3" s="83"/>
-      <c r="G3" s="83"/>
-      <c r="H3" s="83"/>
-      <c r="I3" s="73" t="s">
+      <c r="B3" s="44"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="45"/>
+      <c r="G3" s="45"/>
+      <c r="H3" s="45"/>
+      <c r="I3" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="73"/>
-      <c r="K3" s="73"/>
-      <c r="L3" s="73"/>
-      <c r="M3" s="73"/>
-      <c r="N3" s="73"/>
-      <c r="O3" s="70"/>
-      <c r="P3" s="70"/>
-      <c r="Q3" s="70"/>
-      <c r="R3" s="70"/>
-      <c r="S3" s="70"/>
-      <c r="T3" s="70"/>
-      <c r="U3" s="70"/>
-      <c r="V3" s="70"/>
-      <c r="W3" s="70"/>
-      <c r="X3" s="70"/>
-      <c r="Y3" s="70"/>
-      <c r="Z3" s="70"/>
-      <c r="AA3" s="80"/>
-      <c r="AB3" s="80"/>
-      <c r="AC3" s="80"/>
-      <c r="AD3" s="80"/>
-      <c r="AE3" s="80"/>
-      <c r="AF3" s="80"/>
-      <c r="AG3" s="80"/>
-      <c r="AH3" s="80"/>
-      <c r="AI3" s="80"/>
+      <c r="J3" s="38"/>
+      <c r="K3" s="38"/>
+      <c r="L3" s="38"/>
+      <c r="M3" s="38"/>
+      <c r="N3" s="38"/>
+      <c r="O3" s="41"/>
+      <c r="P3" s="41"/>
+      <c r="Q3" s="41"/>
+      <c r="R3" s="41"/>
+      <c r="S3" s="41"/>
+      <c r="T3" s="41"/>
+      <c r="U3" s="41"/>
+      <c r="V3" s="41"/>
+      <c r="W3" s="41"/>
+      <c r="X3" s="41"/>
+      <c r="Y3" s="41"/>
+      <c r="Z3" s="41"/>
+      <c r="AA3" s="40"/>
+      <c r="AB3" s="40"/>
+      <c r="AC3" s="40"/>
+      <c r="AD3" s="40"/>
+      <c r="AE3" s="40"/>
+      <c r="AF3" s="40"/>
+      <c r="AG3" s="40"/>
+      <c r="AH3" s="40"/>
+      <c r="AI3" s="40"/>
     </row>
-    <row r="4" spans="1:35" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="71" t="s">
+    <row r="4" spans="1:35" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="71"/>
-      <c r="C4" s="72"/>
-      <c r="D4" s="72"/>
-      <c r="E4" s="72"/>
-      <c r="F4" s="72"/>
-      <c r="G4" s="72"/>
-      <c r="H4" s="72"/>
-      <c r="I4" s="73" t="s">
+      <c r="B4" s="44"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="39"/>
+      <c r="H4" s="39"/>
+      <c r="I4" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="J4" s="73"/>
-      <c r="K4" s="73"/>
-      <c r="L4" s="73"/>
-      <c r="M4" s="73"/>
-      <c r="N4" s="73"/>
-      <c r="O4" s="37"/>
-      <c r="P4" s="38"/>
-      <c r="Q4" s="38"/>
-      <c r="R4" s="38"/>
-      <c r="S4" s="38"/>
-      <c r="T4" s="38"/>
-      <c r="U4" s="38"/>
-      <c r="V4" s="38"/>
-      <c r="W4" s="38"/>
-      <c r="X4" s="38"/>
-      <c r="Y4" s="38"/>
-      <c r="Z4" s="39"/>
-      <c r="AA4" s="80"/>
-      <c r="AB4" s="80"/>
-      <c r="AC4" s="80"/>
-      <c r="AD4" s="80"/>
-      <c r="AE4" s="80"/>
-      <c r="AF4" s="80"/>
-      <c r="AG4" s="80"/>
-      <c r="AH4" s="80"/>
-      <c r="AI4" s="80"/>
+      <c r="J4" s="38"/>
+      <c r="K4" s="38"/>
+      <c r="L4" s="38"/>
+      <c r="M4" s="38"/>
+      <c r="N4" s="38"/>
+      <c r="O4" s="68"/>
+      <c r="P4" s="69"/>
+      <c r="Q4" s="69"/>
+      <c r="R4" s="69"/>
+      <c r="S4" s="69"/>
+      <c r="T4" s="69"/>
+      <c r="U4" s="69"/>
+      <c r="V4" s="69"/>
+      <c r="W4" s="69"/>
+      <c r="X4" s="69"/>
+      <c r="Y4" s="69"/>
+      <c r="Z4" s="70"/>
+      <c r="AA4" s="40"/>
+      <c r="AB4" s="40"/>
+      <c r="AC4" s="40"/>
+      <c r="AD4" s="40"/>
+      <c r="AE4" s="40"/>
+      <c r="AF4" s="40"/>
+      <c r="AG4" s="40"/>
+      <c r="AH4" s="40"/>
+      <c r="AI4" s="40"/>
     </row>
-    <row r="5" spans="1:35" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A5" s="27" t="s">
+    <row r="5" spans="1:35" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="66"/>
-      <c r="C5" s="67"/>
-      <c r="D5" s="28">
+      <c r="B5" s="86" t="s">
+        <v>77</v>
+      </c>
+      <c r="C5" s="87"/>
+      <c r="D5" s="27">
         <v>1</v>
       </c>
-      <c r="E5" s="28">
+      <c r="E5" s="27">
         <v>2</v>
       </c>
-      <c r="F5" s="28">
+      <c r="F5" s="27">
         <v>3</v>
       </c>
-      <c r="G5" s="28">
+      <c r="G5" s="27">
         <v>4</v>
       </c>
-      <c r="H5" s="28">
+      <c r="H5" s="27">
         <v>5</v>
       </c>
-      <c r="I5" s="28">
+      <c r="I5" s="27">
         <v>6</v>
       </c>
-      <c r="J5" s="28">
+      <c r="J5" s="27">
         <v>7</v>
       </c>
-      <c r="K5" s="28">
+      <c r="K5" s="27">
         <v>8</v>
       </c>
-      <c r="L5" s="28">
+      <c r="L5" s="27">
         <v>9</v>
       </c>
-      <c r="M5" s="28">
+      <c r="M5" s="27">
         <v>10</v>
       </c>
-      <c r="N5" s="28">
+      <c r="N5" s="27">
         <v>11</v>
       </c>
-      <c r="O5" s="28">
+      <c r="O5" s="27">
         <v>12</v>
       </c>
-      <c r="P5" s="28">
+      <c r="P5" s="27">
         <v>13</v>
       </c>
-      <c r="Q5" s="28">
+      <c r="Q5" s="27">
         <v>14</v>
       </c>
-      <c r="R5" s="28">
+      <c r="R5" s="27">
         <v>15</v>
       </c>
-      <c r="S5" s="28">
+      <c r="S5" s="27">
         <v>16</v>
       </c>
-      <c r="T5" s="28">
+      <c r="T5" s="27">
         <v>17</v>
       </c>
-      <c r="U5" s="28">
+      <c r="U5" s="27">
         <v>18</v>
       </c>
-      <c r="V5" s="28">
+      <c r="V5" s="27">
         <v>19</v>
       </c>
-      <c r="W5" s="28">
+      <c r="W5" s="27">
         <v>20</v>
       </c>
-      <c r="X5" s="28">
+      <c r="X5" s="27">
         <v>21</v>
       </c>
-      <c r="Y5" s="28">
+      <c r="Y5" s="27">
         <v>22</v>
       </c>
-      <c r="Z5" s="28">
+      <c r="Z5" s="27">
         <v>23</v>
       </c>
-      <c r="AA5" s="28">
+      <c r="AA5" s="27">
         <v>24</v>
       </c>
-      <c r="AB5" s="28">
+      <c r="AB5" s="27">
         <v>25</v>
       </c>
-      <c r="AC5" s="28">
+      <c r="AC5" s="27">
         <v>26</v>
       </c>
-      <c r="AD5" s="28">
+      <c r="AD5" s="27">
         <v>27</v>
       </c>
-      <c r="AE5" s="28">
+      <c r="AE5" s="27">
         <v>28</v>
       </c>
-      <c r="AF5" s="28">
+      <c r="AF5" s="27">
         <v>29</v>
       </c>
-      <c r="AG5" s="28">
+      <c r="AG5" s="27">
         <v>30</v>
       </c>
-      <c r="AH5" s="28">
+      <c r="AH5" s="27">
         <v>31</v>
       </c>
-      <c r="AI5" s="29" t="s">
+      <c r="AI5" s="28" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:35" ht="54" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="44">
+    <row r="6" spans="1:35" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="77">
         <v>1</v>
       </c>
-      <c r="B6" s="68" t="s">
+      <c r="B6" s="78" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="69"/>
+      <c r="C6" s="79"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
@@ -2863,16 +2893,16 @@
       <c r="AC6" s="3"/>
       <c r="AD6" s="3"/>
       <c r="AE6" s="3"/>
-      <c r="AF6" s="24"/>
-      <c r="AG6" s="24"/>
-      <c r="AH6" s="24"/>
+      <c r="AF6" s="23"/>
+      <c r="AG6" s="23"/>
+      <c r="AH6" s="23"/>
     </row>
-    <row r="7" spans="1:35" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="60"/>
-      <c r="B7" s="68" t="s">
+    <row r="7" spans="1:35" ht="45.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="80"/>
+      <c r="B7" s="78" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="69"/>
+      <c r="C7" s="79"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
@@ -2901,16 +2931,16 @@
       <c r="AC7" s="3"/>
       <c r="AD7" s="3"/>
       <c r="AE7" s="4"/>
-      <c r="AF7" s="25"/>
-      <c r="AG7" s="25"/>
-      <c r="AH7" s="25"/>
+      <c r="AF7" s="24"/>
+      <c r="AG7" s="24"/>
+      <c r="AH7" s="24"/>
     </row>
-    <row r="8" spans="1:35" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="45"/>
-      <c r="B8" s="68" t="s">
+    <row r="8" spans="1:35" ht="57.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="81"/>
+      <c r="B8" s="78" t="s">
         <v>73</v>
       </c>
-      <c r="C8" s="69"/>
+      <c r="C8" s="79"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
@@ -2939,22 +2969,22 @@
       <c r="AC8" s="3"/>
       <c r="AD8" s="3"/>
       <c r="AE8" s="4"/>
-      <c r="AF8" s="25"/>
-      <c r="AG8" s="25"/>
-      <c r="AH8" s="25"/>
-      <c r="AI8" s="30">
+      <c r="AF8" s="24"/>
+      <c r="AG8" s="24"/>
+      <c r="AH8" s="24"/>
+      <c r="AI8" s="29">
         <f>SUM(D8:AH8)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:35" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:35" ht="65.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="18">
         <v>2</v>
       </c>
-      <c r="B9" s="48" t="s">
+      <c r="B9" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="49"/>
+      <c r="C9" s="47"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
@@ -2983,22 +3013,22 @@
       <c r="AC9" s="3"/>
       <c r="AD9" s="3"/>
       <c r="AE9" s="4"/>
-      <c r="AF9" s="25"/>
-      <c r="AG9" s="25"/>
-      <c r="AH9" s="25"/>
-      <c r="AI9" s="30">
+      <c r="AF9" s="24"/>
+      <c r="AG9" s="24"/>
+      <c r="AH9" s="24"/>
+      <c r="AI9" s="29">
         <f>SUM(D9:AH9)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:35" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="23">
+    <row r="10" spans="1:35" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="82">
         <v>3</v>
       </c>
-      <c r="B10" s="57" t="s">
+      <c r="B10" s="83" t="s">
         <v>74</v>
       </c>
-      <c r="C10" s="58"/>
+      <c r="C10" s="84"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
@@ -3027,22 +3057,22 @@
       <c r="AC10" s="3"/>
       <c r="AD10" s="3"/>
       <c r="AE10" s="4"/>
-      <c r="AF10" s="25"/>
-      <c r="AG10" s="25"/>
-      <c r="AH10" s="25"/>
-      <c r="AI10" s="30">
+      <c r="AF10" s="24"/>
+      <c r="AG10" s="24"/>
+      <c r="AH10" s="24"/>
+      <c r="AI10" s="29">
         <f>SUM(D10:AH10)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:35" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:35" ht="64.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="18">
         <v>4</v>
       </c>
-      <c r="B11" s="59" t="s">
+      <c r="B11" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="49"/>
+      <c r="C11" s="47"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
@@ -3071,15 +3101,15 @@
       <c r="AC11" s="3"/>
       <c r="AD11" s="3"/>
       <c r="AE11" s="6"/>
-      <c r="AF11" s="26"/>
-      <c r="AG11" s="26"/>
-      <c r="AH11" s="26"/>
+      <c r="AF11" s="25"/>
+      <c r="AG11" s="25"/>
+      <c r="AH11" s="25"/>
     </row>
-    <row r="12" spans="1:35" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="44">
+    <row r="12" spans="1:35" ht="51.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="48">
         <v>5</v>
       </c>
-      <c r="B12" s="46" t="s">
+      <c r="B12" s="52" t="s">
         <v>17</v>
       </c>
       <c r="C12" s="22" t="s">
@@ -3113,13 +3143,13 @@
       <c r="AC12" s="3"/>
       <c r="AD12" s="3"/>
       <c r="AE12" s="4"/>
-      <c r="AF12" s="25"/>
-      <c r="AG12" s="25"/>
-      <c r="AH12" s="25"/>
+      <c r="AF12" s="24"/>
+      <c r="AG12" s="24"/>
+      <c r="AH12" s="24"/>
     </row>
-    <row r="13" spans="1:35" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="60"/>
-      <c r="B13" s="61"/>
+    <row r="13" spans="1:35" ht="45.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="49"/>
+      <c r="B13" s="53"/>
       <c r="C13" s="21" t="s">
         <v>19</v>
       </c>
@@ -3151,13 +3181,13 @@
       <c r="AC13" s="3"/>
       <c r="AD13" s="3"/>
       <c r="AE13" s="4"/>
-      <c r="AF13" s="25"/>
-      <c r="AG13" s="25"/>
-      <c r="AH13" s="25"/>
+      <c r="AF13" s="24"/>
+      <c r="AG13" s="24"/>
+      <c r="AH13" s="24"/>
     </row>
-    <row r="14" spans="1:35" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="60"/>
-      <c r="B14" s="61"/>
+    <row r="14" spans="1:35" ht="41.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="49"/>
+      <c r="B14" s="53"/>
       <c r="C14" s="21" t="s">
         <v>20</v>
       </c>
@@ -3189,17 +3219,17 @@
       <c r="AC14" s="3"/>
       <c r="AD14" s="3"/>
       <c r="AE14" s="4"/>
-      <c r="AF14" s="25"/>
-      <c r="AG14" s="25"/>
-      <c r="AH14" s="25"/>
-      <c r="AI14" s="30">
+      <c r="AF14" s="24"/>
+      <c r="AG14" s="24"/>
+      <c r="AH14" s="24"/>
+      <c r="AI14" s="29">
         <f t="shared" ref="AI14:AI20" si="0">SUM(D14:AH14)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:35" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="45"/>
-      <c r="B15" s="47"/>
+    <row r="15" spans="1:35" ht="56.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="50"/>
+      <c r="B15" s="54"/>
       <c r="C15" s="21" t="s">
         <v>21</v>
       </c>
@@ -3231,15 +3261,15 @@
       <c r="AC15" s="3"/>
       <c r="AD15" s="3"/>
       <c r="AE15" s="6"/>
-      <c r="AF15" s="26"/>
-      <c r="AG15" s="26"/>
-      <c r="AH15" s="26"/>
+      <c r="AF15" s="25"/>
+      <c r="AG15" s="25"/>
+      <c r="AH15" s="25"/>
     </row>
-    <row r="16" spans="1:35" ht="54" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="62">
+    <row r="16" spans="1:35" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="55">
         <v>6</v>
       </c>
-      <c r="B16" s="64" t="s">
+      <c r="B16" s="57" t="s">
         <v>22</v>
       </c>
       <c r="C16" s="19" t="s">
@@ -3273,13 +3303,13 @@
       <c r="AC16" s="3"/>
       <c r="AD16" s="3"/>
       <c r="AE16" s="6"/>
-      <c r="AF16" s="26"/>
-      <c r="AG16" s="26"/>
-      <c r="AH16" s="26"/>
+      <c r="AF16" s="25"/>
+      <c r="AG16" s="25"/>
+      <c r="AH16" s="25"/>
     </row>
-    <row r="17" spans="1:35" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="63"/>
-      <c r="B17" s="65"/>
+    <row r="17" spans="1:35" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="56"/>
+      <c r="B17" s="58"/>
       <c r="C17" s="20" t="s">
         <v>24</v>
       </c>
@@ -3311,19 +3341,19 @@
       <c r="AC17" s="3"/>
       <c r="AD17" s="3"/>
       <c r="AE17" s="4"/>
-      <c r="AF17" s="25"/>
-      <c r="AG17" s="25"/>
-      <c r="AH17" s="25"/>
-      <c r="AI17" s="30">
+      <c r="AF17" s="24"/>
+      <c r="AG17" s="24"/>
+      <c r="AH17" s="24"/>
+      <c r="AI17" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:35" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="44">
+    <row r="18" spans="1:35" ht="42" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="48">
         <v>7</v>
       </c>
-      <c r="B18" s="46" t="s">
+      <c r="B18" s="52" t="s">
         <v>25</v>
       </c>
       <c r="C18" s="21" t="s">
@@ -3357,13 +3387,13 @@
       <c r="AC18" s="3"/>
       <c r="AD18" s="3"/>
       <c r="AE18" s="6"/>
-      <c r="AF18" s="26"/>
-      <c r="AG18" s="26"/>
-      <c r="AH18" s="26"/>
+      <c r="AF18" s="25"/>
+      <c r="AG18" s="25"/>
+      <c r="AH18" s="25"/>
     </row>
-    <row r="19" spans="1:35" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="45"/>
-      <c r="B19" s="47"/>
+    <row r="19" spans="1:35" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="50"/>
+      <c r="B19" s="54"/>
       <c r="C19" s="21" t="s">
         <v>24</v>
       </c>
@@ -3395,22 +3425,22 @@
       <c r="AC19" s="3"/>
       <c r="AD19" s="3"/>
       <c r="AE19" s="4"/>
-      <c r="AF19" s="25"/>
-      <c r="AG19" s="25"/>
-      <c r="AH19" s="25"/>
-      <c r="AI19" s="30">
+      <c r="AF19" s="24"/>
+      <c r="AG19" s="24"/>
+      <c r="AH19" s="24"/>
+      <c r="AI19" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:35" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:35" ht="73.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="18">
         <v>8</v>
       </c>
-      <c r="B20" s="48" t="s">
+      <c r="B20" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="C20" s="49"/>
+      <c r="C20" s="47"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
@@ -3439,15 +3469,15 @@
       <c r="AC20" s="3"/>
       <c r="AD20" s="3"/>
       <c r="AE20" s="4"/>
-      <c r="AF20" s="25"/>
-      <c r="AG20" s="25"/>
-      <c r="AH20" s="25"/>
-      <c r="AI20" s="30">
+      <c r="AF20" s="24"/>
+      <c r="AG20" s="24"/>
+      <c r="AH20" s="24"/>
+      <c r="AI20" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:35" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A21" s="7"/>
       <c r="B21" s="8"/>
       <c r="C21" s="7"/>
@@ -3484,46 +3514,46 @@
       <c r="AH21" s="7"/>
       <c r="AI21" s="9"/>
     </row>
-    <row r="22" spans="1:35" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A22" s="7"/>
       <c r="B22" s="8"/>
       <c r="C22" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D22" s="50"/>
-      <c r="E22" s="51"/>
-      <c r="F22" s="51"/>
-      <c r="G22" s="51"/>
-      <c r="H22" s="51"/>
-      <c r="I22" s="51"/>
-      <c r="J22" s="51"/>
-      <c r="K22" s="51"/>
-      <c r="L22" s="51"/>
-      <c r="M22" s="51"/>
-      <c r="N22" s="51"/>
-      <c r="O22" s="51"/>
-      <c r="P22" s="51"/>
-      <c r="Q22" s="51"/>
-      <c r="R22" s="51"/>
-      <c r="S22" s="51"/>
-      <c r="T22" s="51"/>
-      <c r="U22" s="51"/>
-      <c r="V22" s="51"/>
-      <c r="W22" s="51"/>
-      <c r="X22" s="51"/>
-      <c r="Y22" s="51"/>
-      <c r="Z22" s="51"/>
-      <c r="AA22" s="51"/>
-      <c r="AB22" s="51"/>
-      <c r="AC22" s="51"/>
-      <c r="AD22" s="51"/>
-      <c r="AE22" s="51"/>
-      <c r="AF22" s="51"/>
-      <c r="AG22" s="51"/>
-      <c r="AH22" s="51"/>
-      <c r="AI22" s="52"/>
+      <c r="D22" s="61"/>
+      <c r="E22" s="62"/>
+      <c r="F22" s="62"/>
+      <c r="G22" s="62"/>
+      <c r="H22" s="62"/>
+      <c r="I22" s="62"/>
+      <c r="J22" s="62"/>
+      <c r="K22" s="62"/>
+      <c r="L22" s="62"/>
+      <c r="M22" s="62"/>
+      <c r="N22" s="62"/>
+      <c r="O22" s="62"/>
+      <c r="P22" s="62"/>
+      <c r="Q22" s="62"/>
+      <c r="R22" s="62"/>
+      <c r="S22" s="62"/>
+      <c r="T22" s="62"/>
+      <c r="U22" s="62"/>
+      <c r="V22" s="62"/>
+      <c r="W22" s="62"/>
+      <c r="X22" s="62"/>
+      <c r="Y22" s="62"/>
+      <c r="Z22" s="62"/>
+      <c r="AA22" s="62"/>
+      <c r="AB22" s="62"/>
+      <c r="AC22" s="62"/>
+      <c r="AD22" s="62"/>
+      <c r="AE22" s="62"/>
+      <c r="AF22" s="62"/>
+      <c r="AG22" s="62"/>
+      <c r="AH22" s="62"/>
+      <c r="AI22" s="63"/>
     </row>
-    <row r="23" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A23" s="9"/>
       <c r="B23" s="11"/>
       <c r="C23" s="12"/>
@@ -3560,40 +3590,40 @@
       <c r="AH23" s="9"/>
       <c r="AI23" s="9"/>
     </row>
-    <row r="24" spans="1:35" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:35" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="9"/>
       <c r="B24" s="11"/>
       <c r="C24" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D24" s="31" t="s">
+      <c r="D24" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="E24" s="53" t="s">
+      <c r="E24" s="64" t="s">
         <v>29</v>
       </c>
-      <c r="F24" s="53"/>
-      <c r="G24" s="54"/>
-      <c r="H24" s="31" t="s">
+      <c r="F24" s="64"/>
+      <c r="G24" s="65"/>
+      <c r="H24" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="I24" s="55" t="s">
+      <c r="I24" s="66" t="s">
         <v>30</v>
       </c>
-      <c r="J24" s="55"/>
-      <c r="K24" s="55"/>
-      <c r="L24" s="55"/>
-      <c r="M24" s="55"/>
-      <c r="N24" s="55"/>
-      <c r="O24" s="56"/>
-      <c r="P24" s="31" t="s">
+      <c r="J24" s="66"/>
+      <c r="K24" s="66"/>
+      <c r="L24" s="66"/>
+      <c r="M24" s="66"/>
+      <c r="N24" s="66"/>
+      <c r="O24" s="67"/>
+      <c r="P24" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="Q24" s="53" t="s">
+      <c r="Q24" s="64" t="s">
         <v>32</v>
       </c>
-      <c r="R24" s="53"/>
-      <c r="S24" s="54"/>
+      <c r="R24" s="64"/>
+      <c r="S24" s="65"/>
       <c r="T24" s="9"/>
       <c r="U24" s="9"/>
       <c r="V24" s="9"/>
@@ -3611,192 +3641,192 @@
       <c r="AH24" s="9"/>
       <c r="AI24" s="9"/>
     </row>
-    <row r="25" spans="1:35" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:35" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="9"/>
       <c r="B25" s="11"/>
       <c r="C25" s="11"/>
-      <c r="D25" s="31" t="s">
+      <c r="D25" s="30" t="s">
         <v>75</v>
       </c>
-      <c r="E25" s="33" t="s">
+      <c r="E25" s="73" t="s">
         <v>33</v>
       </c>
-      <c r="F25" s="33"/>
-      <c r="G25" s="36"/>
-      <c r="H25" s="32" t="s">
+      <c r="F25" s="73"/>
+      <c r="G25" s="74"/>
+      <c r="H25" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="I25" s="42" t="s">
+      <c r="I25" s="75" t="s">
         <v>35</v>
       </c>
-      <c r="J25" s="42"/>
-      <c r="K25" s="43"/>
+      <c r="J25" s="75"/>
+      <c r="K25" s="76"/>
       <c r="L25" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="M25" s="34" t="s">
+      <c r="M25" s="59" t="s">
         <v>37</v>
       </c>
-      <c r="N25" s="34"/>
-      <c r="O25" s="35"/>
+      <c r="N25" s="59"/>
+      <c r="O25" s="60"/>
       <c r="P25" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="Q25" s="34" t="s">
+      <c r="Q25" s="59" t="s">
         <v>39</v>
       </c>
-      <c r="R25" s="34"/>
-      <c r="S25" s="35"/>
+      <c r="R25" s="59"/>
+      <c r="S25" s="60"/>
       <c r="T25" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="U25" s="34" t="s">
+      <c r="U25" s="59" t="s">
         <v>41</v>
       </c>
-      <c r="V25" s="34"/>
-      <c r="W25" s="35"/>
+      <c r="V25" s="59"/>
+      <c r="W25" s="60"/>
       <c r="X25" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="Y25" s="34" t="s">
+      <c r="Y25" s="59" t="s">
         <v>43</v>
       </c>
-      <c r="Z25" s="34"/>
-      <c r="AA25" s="35"/>
+      <c r="Z25" s="59"/>
+      <c r="AA25" s="60"/>
       <c r="AB25" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="AC25" s="34" t="s">
+      <c r="AC25" s="59" t="s">
         <v>45</v>
       </c>
-      <c r="AD25" s="34"/>
-      <c r="AE25" s="35"/>
+      <c r="AD25" s="59"/>
+      <c r="AE25" s="60"/>
       <c r="AF25" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="AG25" s="34" t="s">
+      <c r="AG25" s="59" t="s">
         <v>47</v>
       </c>
-      <c r="AH25" s="34"/>
-      <c r="AI25" s="35"/>
+      <c r="AH25" s="59"/>
+      <c r="AI25" s="60"/>
     </row>
-    <row r="26" spans="1:35" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:35" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="9"/>
       <c r="B26" s="11"/>
       <c r="C26" s="11"/>
       <c r="D26" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="E26" s="34" t="s">
+      <c r="E26" s="59" t="s">
         <v>48</v>
       </c>
-      <c r="F26" s="34"/>
-      <c r="G26" s="35"/>
+      <c r="F26" s="59"/>
+      <c r="G26" s="60"/>
       <c r="H26" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="I26" s="40" t="s">
+      <c r="I26" s="71" t="s">
         <v>50</v>
       </c>
-      <c r="J26" s="40"/>
-      <c r="K26" s="41"/>
+      <c r="J26" s="71"/>
+      <c r="K26" s="72"/>
       <c r="L26" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="M26" s="34" t="s">
+      <c r="M26" s="59" t="s">
         <v>52</v>
       </c>
-      <c r="N26" s="34"/>
-      <c r="O26" s="35"/>
+      <c r="N26" s="59"/>
+      <c r="O26" s="60"/>
       <c r="P26" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="Q26" s="34" t="s">
+      <c r="Q26" s="59" t="s">
         <v>54</v>
       </c>
-      <c r="R26" s="34"/>
-      <c r="S26" s="35"/>
+      <c r="R26" s="59"/>
+      <c r="S26" s="60"/>
       <c r="T26" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="U26" s="34" t="s">
+      <c r="U26" s="59" t="s">
         <v>56</v>
       </c>
-      <c r="V26" s="34"/>
-      <c r="W26" s="35"/>
+      <c r="V26" s="59"/>
+      <c r="W26" s="60"/>
       <c r="X26" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="Y26" s="34" t="s">
+      <c r="Y26" s="59" t="s">
         <v>58</v>
       </c>
-      <c r="Z26" s="34"/>
-      <c r="AA26" s="35"/>
+      <c r="Z26" s="59"/>
+      <c r="AA26" s="60"/>
       <c r="AB26" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="AC26" s="33" t="s">
+      <c r="AC26" s="73" t="s">
         <v>60</v>
       </c>
-      <c r="AD26" s="33"/>
-      <c r="AE26" s="36"/>
+      <c r="AD26" s="73"/>
+      <c r="AE26" s="74"/>
       <c r="AF26" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="AG26" s="33" t="s">
+      <c r="AG26" s="73" t="s">
         <v>62</v>
       </c>
-      <c r="AH26" s="33"/>
-      <c r="AI26" s="36"/>
+      <c r="AH26" s="73"/>
+      <c r="AI26" s="74"/>
     </row>
-    <row r="27" spans="1:35" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:35" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="9"/>
       <c r="B27" s="11"/>
       <c r="C27" s="11"/>
       <c r="D27" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="E27" s="33" t="s">
+      <c r="E27" s="73" t="s">
         <v>64</v>
       </c>
-      <c r="F27" s="33"/>
-      <c r="G27" s="33"/>
+      <c r="F27" s="73"/>
+      <c r="G27" s="73"/>
       <c r="H27" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="I27" s="34" t="s">
+      <c r="I27" s="59" t="s">
         <v>66</v>
       </c>
-      <c r="J27" s="34"/>
-      <c r="K27" s="34"/>
-      <c r="L27" s="34"/>
-      <c r="M27" s="34"/>
-      <c r="N27" s="34"/>
-      <c r="O27" s="35"/>
+      <c r="J27" s="59"/>
+      <c r="K27" s="59"/>
+      <c r="L27" s="59"/>
+      <c r="M27" s="59"/>
+      <c r="N27" s="59"/>
+      <c r="O27" s="60"/>
       <c r="P27" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="Q27" s="33" t="s">
+      <c r="Q27" s="73" t="s">
         <v>68</v>
       </c>
-      <c r="R27" s="33"/>
-      <c r="S27" s="36"/>
+      <c r="R27" s="73"/>
+      <c r="S27" s="74"/>
       <c r="T27" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="U27" s="33" t="s">
+      <c r="U27" s="73" t="s">
         <v>70</v>
       </c>
-      <c r="V27" s="33"/>
-      <c r="W27" s="36"/>
+      <c r="V27" s="73"/>
+      <c r="W27" s="74"/>
       <c r="X27" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="Y27" s="33" t="s">
+      <c r="Y27" s="73" t="s">
         <v>72</v>
       </c>
-      <c r="Z27" s="33"/>
-      <c r="AA27" s="36"/>
+      <c r="Z27" s="73"/>
+      <c r="AA27" s="74"/>
       <c r="AB27" s="9"/>
       <c r="AC27" s="9"/>
       <c r="AD27" s="9"/>
@@ -3806,8 +3836,57 @@
       <c r="AH27" s="9"/>
       <c r="AI27" s="9"/>
     </row>
+    <row r="29" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="D29" s="85"/>
+      <c r="E29" s="85"/>
+    </row>
   </sheetData>
   <mergeCells count="55">
+    <mergeCell ref="E27:G27"/>
+    <mergeCell ref="I27:O27"/>
+    <mergeCell ref="Q27:S27"/>
+    <mergeCell ref="U27:W27"/>
+    <mergeCell ref="Y27:AA27"/>
+    <mergeCell ref="Y26:AA26"/>
+    <mergeCell ref="AC26:AE26"/>
+    <mergeCell ref="AG26:AI26"/>
+    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="I25:K25"/>
+    <mergeCell ref="M25:O25"/>
+    <mergeCell ref="Q25:S25"/>
+    <mergeCell ref="U25:W25"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="I26:K26"/>
+    <mergeCell ref="M26:O26"/>
+    <mergeCell ref="Q26:S26"/>
+    <mergeCell ref="U26:W26"/>
+    <mergeCell ref="Y25:AA25"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="D22:AI22"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="I24:O24"/>
+    <mergeCell ref="Q24:S24"/>
+    <mergeCell ref="AC25:AE25"/>
+    <mergeCell ref="AG25:AI25"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="B12:B15"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="O3:Z3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:H4"/>
+    <mergeCell ref="I4:N4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="O4:Z4"/>
     <mergeCell ref="A1:H2"/>
     <mergeCell ref="I1:N1"/>
     <mergeCell ref="O1:Z1"/>
@@ -3818,79 +3897,34 @@
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="C3:H3"/>
     <mergeCell ref="I3:N3"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="O3:Z3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:H4"/>
-    <mergeCell ref="I4:N4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="A12:A15"/>
-    <mergeCell ref="B12:B15"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="Y25:AA25"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="D22:AI22"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="I24:O24"/>
-    <mergeCell ref="Q24:S24"/>
-    <mergeCell ref="O4:Z4"/>
-    <mergeCell ref="AC25:AE25"/>
-    <mergeCell ref="AG25:AI25"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="I26:K26"/>
-    <mergeCell ref="M26:O26"/>
-    <mergeCell ref="Q26:S26"/>
-    <mergeCell ref="U26:W26"/>
-    <mergeCell ref="Y26:AA26"/>
-    <mergeCell ref="AC26:AE26"/>
-    <mergeCell ref="AG26:AI26"/>
-    <mergeCell ref="E25:G25"/>
-    <mergeCell ref="I25:K25"/>
-    <mergeCell ref="M25:O25"/>
-    <mergeCell ref="Q25:S25"/>
-    <mergeCell ref="U25:W25"/>
-    <mergeCell ref="E27:G27"/>
-    <mergeCell ref="I27:O27"/>
-    <mergeCell ref="Q27:S27"/>
-    <mergeCell ref="U27:W27"/>
-    <mergeCell ref="Y27:AA27"/>
   </mergeCells>
   <conditionalFormatting sqref="A1 I1:I4 O1:O4 A3:A4 C3:C4 D23:M23 X25:Y25 D26:D27 T26:Y27">
-    <cfRule type="cellIs" dxfId="133" priority="114" operator="equal">
-      <formula>"ZWO"</formula>
+    <cfRule type="cellIs" dxfId="133" priority="112" operator="equal">
+      <formula>"ŚWREH"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="132" priority="113" operator="equal">
       <formula>"ŚWREH"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="131" priority="112" operator="equal">
-      <formula>"ŚWREH"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="130" priority="120" operator="equal">
+    <cfRule type="cellIs" dxfId="131" priority="114" operator="equal">
+      <formula>"ZWO"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="130" priority="115" operator="equal">
+      <formula>"ZWL"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="129" priority="116" operator="equal">
+      <formula>"UWŻ"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="128" priority="117" operator="equal">
+      <formula>"UW"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="127" priority="118" operator="equal">
+      <formula>"WN"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="126" priority="119" operator="equal">
+      <formula>"WN"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="125" priority="120" operator="equal">
       <formula>"WD"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="129" priority="119" operator="equal">
-      <formula>"WN"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="128" priority="118" operator="equal">
-      <formula>"WN"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="127" priority="117" operator="equal">
-      <formula>"UW"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="126" priority="116" operator="equal">
-      <formula>"UWŻ"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="125" priority="115" operator="equal">
-      <formula>"ZWL"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1 I1:I4 O1:O4 A3:A4 C3:C4 D23:M23 X25:Y25 T26:Y27">
@@ -3899,23 +3933,23 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1 I1:I4 O1:O4 W2:X2 A3:A4 C3:C4">
-    <cfRule type="cellIs" dxfId="123" priority="106" operator="equal">
+    <cfRule type="cellIs" dxfId="123" priority="105" operator="equal">
+      <formula>"UWŻ"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="122" priority="106" operator="equal">
       <formula>"UW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="122" priority="107" operator="equal">
+    <cfRule type="cellIs" dxfId="121" priority="107" operator="equal">
       <formula>"ZWO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="121" priority="108" operator="equal">
+    <cfRule type="cellIs" dxfId="120" priority="108" operator="equal">
       <formula>"ZWL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="120" priority="109" operator="equal">
+    <cfRule type="cellIs" dxfId="119" priority="109" operator="equal">
       <formula>"WŚ"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="119" priority="110" operator="equal">
+    <cfRule type="cellIs" dxfId="118" priority="110" operator="equal">
       <formula>"WD"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="118" priority="105" operator="equal">
-      <formula>"UWŻ"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="117" priority="111" operator="equal">
       <formula>"WN"</formula>
@@ -3965,65 +3999,65 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10">
+    <cfRule type="cellIs" dxfId="103" priority="83" operator="equal">
+      <formula>"WN"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="102" priority="84" operator="equal">
+      <formula>"ZW"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="101" priority="85" operator="equal">
+      <formula>"DEL"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="100" priority="86" operator="equal">
+      <formula>"NN"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="99" priority="87" operator="equal">
+      <formula>"NB"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="98" priority="88" operator="equal">
+      <formula>"NP"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="97" priority="89" operator="equal">
+      <formula>"D"</formula>
+    </cfRule>
     <cfRule type="cellIs" priority="90" operator="equal">
       <formula>"WP"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="103" priority="89" operator="equal">
-      <formula>"D"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="102" priority="88" operator="equal">
-      <formula>"NP"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="101" priority="87" operator="equal">
-      <formula>"NB"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="100" priority="86" operator="equal">
-      <formula>"NN"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="99" priority="85" operator="equal">
-      <formula>"DEL"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="98" priority="84" operator="equal">
-      <formula>"ZW"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="97" priority="83" operator="equal">
-      <formula>"WN"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="96" priority="102" operator="equal">
-      <formula>"W5"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="95" priority="104" operator="equal">
-      <formula>"WN"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="94" priority="103" operator="equal">
-      <formula>"WŚ"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="93" priority="99" operator="equal">
-      <formula>"UW"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="92" priority="97" operator="equal">
-      <formula>"UO"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="91" priority="98" operator="equal">
-      <formula>"UW"</formula>
+    <cfRule type="cellIs" dxfId="96" priority="91" operator="equal">
+      <formula>"UB"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="95" priority="92" operator="equal">
+      <formula>"Uwych"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="94" priority="93" operator="equal">
+      <formula>"UR"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="93" priority="94" operator="equal">
+      <formula>"UM"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="92" priority="95" operator="equal">
+      <formula>"UOP"</formula>
     </cfRule>
     <cfRule type="cellIs" priority="96" operator="equal">
       <formula>"UO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="90" priority="95" operator="equal">
-      <formula>"UOP"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="89" priority="94" operator="equal">
-      <formula>"UM"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="88" priority="93" operator="equal">
-      <formula>"UR"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="87" priority="92" operator="equal">
-      <formula>"Uwych"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="86" priority="91" operator="equal">
-      <formula>"UB"</formula>
+    <cfRule type="cellIs" dxfId="91" priority="97" operator="equal">
+      <formula>"UO"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="90" priority="98" operator="equal">
+      <formula>"UW"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="89" priority="99" operator="equal">
+      <formula>"UW"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="88" priority="102" operator="equal">
+      <formula>"W5"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="87" priority="103" operator="equal">
+      <formula>"WŚ"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="86" priority="104" operator="equal">
+      <formula>"WN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22">
@@ -4051,55 +4085,55 @@
     <cfRule type="cellIs" dxfId="78" priority="20" operator="equal">
       <formula>"UW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="77" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="21" operator="equal">
+      <formula>"WN"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="76" priority="22" operator="equal">
+      <formula>"WN"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="75" priority="23" operator="equal">
+      <formula>"WD"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="74" priority="24" operator="equal">
       <formula>"WŚ"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="76" priority="23" operator="equal">
-      <formula>"WD"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="75" priority="22" operator="equal">
-      <formula>"WN"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="74" priority="21" operator="equal">
-      <formula>"WN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24">
-    <cfRule type="cellIs" dxfId="73" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="25" operator="equal">
+      <formula>"WD"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="72" priority="26" operator="equal">
+      <formula>"WD"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="71" priority="27" operator="equal">
       <formula>"ŚWREH"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="72" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="28" operator="equal">
+      <formula>"ŚWREH"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="69" priority="29" operator="equal">
+      <formula>"ZWO"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="68" priority="30" operator="equal">
+      <formula>"ZWL"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="67" priority="31" operator="equal">
+      <formula>"UWŻ"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="66" priority="32" operator="equal">
+      <formula>"UW"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="65" priority="33" operator="equal">
       <formula>"WN"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="71" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="34" operator="equal">
       <formula>"WN"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="70" priority="32" operator="equal">
-      <formula>"UW"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="69" priority="30" operator="equal">
-      <formula>"ZWL"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="35" operator="equal">
+      <formula>"WD"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="62" priority="36" operator="equal">
       <formula>"WŚ"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="67" priority="35" operator="equal">
-      <formula>"WD"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="31" operator="equal">
-      <formula>"UWŻ"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="65" priority="29" operator="equal">
-      <formula>"ZWO"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="27" operator="equal">
-      <formula>"ŚWREH"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="63" priority="26" operator="equal">
-      <formula>"WD"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="25" operator="equal">
-      <formula>"WD"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D23:M23 X25:Y25 AF25:AG26 D26:D27 T26:Y27">
@@ -4116,52 +4150,52 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E18:G18 J18:AH18">
-    <cfRule type="cellIs" dxfId="58" priority="149" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="147" operator="equal">
+      <formula>"OP"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="57" priority="148" operator="equal">
+      <formula>"CH"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="56" priority="149" operator="equal">
       <formula>"UW"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="147" operator="equal">
-      <formula>"OP"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="148" operator="equal">
-      <formula>"CH"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T25:U25">
-    <cfRule type="cellIs" dxfId="55" priority="45" operator="equal">
-      <formula>"WN"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="44" operator="equal">
-      <formula>"UW"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="53" priority="43" operator="equal">
-      <formula>"UWŻ"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="42" operator="equal">
-      <formula>"ZWL"</formula>
+    <cfRule type="cellIs" dxfId="55" priority="37" operator="equal">
+      <formula>"WD"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="54" priority="38" operator="equal">
+      <formula>"WD"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="53" priority="39" operator="equal">
+      <formula>"ŚWREH"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="52" priority="40" operator="equal">
+      <formula>"ŚWREH"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="51" priority="41" operator="equal">
       <formula>"ZWO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="40" operator="equal">
-      <formula>"ŚWREH"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="39" operator="equal">
-      <formula>"ŚWREH"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="38" operator="equal">
-      <formula>"WD"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="37" operator="equal">
-      <formula>"WD"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="48" operator="equal">
-      <formula>"WŚ"</formula>
+    <cfRule type="cellIs" dxfId="50" priority="42" operator="equal">
+      <formula>"ZWL"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="49" priority="43" operator="equal">
+      <formula>"UWŻ"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="48" priority="44" operator="equal">
+      <formula>"UW"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="47" priority="45" operator="equal">
+      <formula>"WN"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="46" priority="46" operator="equal">
+      <formula>"WN"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="45" priority="47" operator="equal">
       <formula>"WD"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="46" operator="equal">
-      <formula>"WN"</formula>
+    <cfRule type="cellIs" dxfId="44" priority="48" operator="equal">
+      <formula>"WŚ"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W2">
@@ -4173,65 +4207,65 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA1 A5:AI5 A6:B6 D6:AH7 B7:B8 D8:AI10 A9:B9 A11:C12 D11:AH13 A13:A15 C13:C15 D14:AI14 D15:AH16 A16:C16 A17 C17:AI17 A18:AH18 A19 C19 D19:AI20 A20:B20 A21:AI21 A22:B22 D22 A23:C23 N23:AI23 A24:B24 T24:AI24 A25:C27 AB27:AH27">
-    <cfRule type="cellIs" dxfId="41" priority="129" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="124" operator="equal">
+      <formula>"WN"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="40" priority="125" operator="equal">
+      <formula>"ZW"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="39" priority="126" operator="equal">
+      <formula>"DEL"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="38" priority="127" operator="equal">
+      <formula>"NN"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="37" priority="128" operator="equal">
+      <formula>"NB"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="36" priority="129" operator="equal">
       <formula>"NP"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="130" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="130" operator="equal">
       <formula>"D"</formula>
     </cfRule>
     <cfRule type="cellIs" priority="131" operator="equal">
       <formula>"WP"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="133" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="132" operator="equal">
+      <formula>"UB"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="33" priority="133" operator="equal">
       <formula>"Uwych"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="134" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="134" operator="equal">
       <formula>"UR"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="135" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="135" operator="equal">
       <formula>"UM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="128" operator="equal">
-      <formula>"NB"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="136" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="136" operator="equal">
       <formula>"UOP"</formula>
     </cfRule>
     <cfRule type="cellIs" priority="137" operator="equal">
       <formula>"UO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="138" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="138" operator="equal">
       <formula>"UO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="139" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="139" operator="equal">
       <formula>"UW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="140" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="140" operator="equal">
       <formula>"UW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="143" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="143" operator="equal">
       <formula>"W5"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="144" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="144" operator="equal">
       <formula>"WŚ"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="145" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="145" operator="equal">
       <formula>"WN"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="132" operator="equal">
-      <formula>"UB"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="124" operator="equal">
-      <formula>"WN"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="125" operator="equal">
-      <formula>"ZW"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="126" operator="equal">
-      <formula>"DEL"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="127" operator="equal">
-      <formula>"NN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA1 B5:AI5 D6:AH7 D8:AI10 B11:C12 D11:AH13 C13:C15 D14:AI14 D15:AH16 B16:C16 C17:AI17 B18:AH18 C19 D19:AI20 B20 B21:AI21 B22 D22 B23:C23 N23:AI23 B24 T24:AI24 B25:C27 AB27:AH27">
@@ -4243,35 +4277,35 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB25:AC26">
-    <cfRule type="cellIs" dxfId="21" priority="58" operator="equal">
-      <formula>"WN"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="57" operator="equal">
-      <formula>"WN"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="56" operator="equal">
-      <formula>"UW"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="55" operator="equal">
-      <formula>"UWŻ"</formula>
+    <cfRule type="cellIs" dxfId="21" priority="49" operator="equal">
+      <formula>"WD"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="20" priority="50" operator="equal">
+      <formula>"WD"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="19" priority="51" operator="equal">
+      <formula>"ŚWREH"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="52" operator="equal">
+      <formula>"ŚWREH"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="17" priority="53" operator="equal">
       <formula>"ZWO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="51" operator="equal">
-      <formula>"ŚWREH"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="50" operator="equal">
-      <formula>"WD"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="49" operator="equal">
-      <formula>"WD"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="52" operator="equal">
-      <formula>"ŚWREH"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="54" operator="equal">
       <formula>"ZWL"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="15" priority="55" operator="equal">
+      <formula>"UWŻ"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="56" operator="equal">
+      <formula>"UW"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="13" priority="57" operator="equal">
+      <formula>"WN"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="58" operator="equal">
+      <formula>"WN"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="11" priority="59" operator="equal">
       <formula>"WD"</formula>
@@ -4281,38 +4315,226 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF25:AG26">
-    <cfRule type="cellIs" dxfId="9" priority="71" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="63" operator="equal">
+      <formula>"ŚWREH"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="64" operator="equal">
+      <formula>"ŚWREH"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="65" operator="equal">
+      <formula>"ZWO"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="66" operator="equal">
+      <formula>"ZWL"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="67" operator="equal">
+      <formula>"UWŻ"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="68" operator="equal">
+      <formula>"UW"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="69" operator="equal">
+      <formula>"WN"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="70" operator="equal">
+      <formula>"WN"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="71" operator="equal">
       <formula>"WD"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="72" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="72" operator="equal">
       <formula>"WŚ"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="70" operator="equal">
-      <formula>"WN"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="69" operator="equal">
-      <formula>"WN"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="68" operator="equal">
-      <formula>"UW"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="66" operator="equal">
-      <formula>"ZWL"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="67" operator="equal">
-      <formula>"UWŻ"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="65" operator="equal">
-      <formula>"ZWO"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="64" operator="equal">
-      <formula>"ŚWREH"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="63" operator="equal">
-      <formula>"ŚWREH"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100EFDF2CCD7F2A9549A796EF6A53171BC0" ma:contentTypeVersion="3" ma:contentTypeDescription="Utwórz nowy dokument." ma:contentTypeScope="" ma:versionID="17fdab98003bcb8b0eb99cbacf57169e">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c61e7320-65a9-489d-8fd8-fad1618a30c1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fb41fdb58a90dd9e596254dbf35bfdcc" ns2:_="">
+    <xsd:import namespace="c61e7320-65a9-489d-8fd8-fad1618a30c1"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="c61e7320-65a9-489d-8fd8-fad1618a30c1" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSearchProperties" ma:index="10" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Typ zawartości"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Tytuł"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4CD4CF01-6166-4398-8732-9E722BD8F723}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5B9BB2D-0FA0-4FA8-93A3-294DB42DB928}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="c61e7320-65a9-489d-8fd8-fad1618a30c1"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6DCF13F3-6C9E-4B19-BFCD-414BC58C8417}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
feat(overtime): update overtime template
</commit_message>
<xml_diff>
--- a/src/assets/overtime_template.xlsx
+++ b/src/assets/overtime_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bbcgroup365.sharepoint.com/sites/CEP-O-OgolnePL-HR/Shared Documents/HR/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="27" documentId="13_ncr:1_{4853A9B9-1D28-4D7F-B792-A1A904D0EE10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EDDCF0AE-9EEC-4C5F-81C2-C0732B928168}"/>
+  <xr:revisionPtr revIDLastSave="30" documentId="13_ncr:1_{4853A9B9-1D28-4D7F-B792-A1A904D0EE10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{65D3C8FA-6DC0-414B-A25A-7F9F72589715}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{5C54F8F0-E29B-4B1D-B5B0-84E7A0453ECD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{5C54F8F0-E29B-4B1D-B5B0-84E7A0453ECD}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="81">
   <si>
     <t>MIESIĘCZNA 
 KARTA EWIDENCJI CZASU PRACY</t>
@@ -404,6 +404,15 @@
     <t>żółte wiersze do uzupełnienia obowiązkowo
 pozostałe opcjonalnie</t>
   </si>
+  <si>
+    <t>SOBOTA</t>
+  </si>
+  <si>
+    <t>NIEDZIELA</t>
+  </si>
+  <si>
+    <t>ŚWIĘTO</t>
+  </si>
 </sst>
 </file>
 
@@ -412,7 +421,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="h:mm;@"/>
   </numFmts>
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -595,8 +604,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -636,6 +653,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF5C58C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF8CF5C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF5CC0FF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -803,7 +838,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -898,6 +933,141 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -916,153 +1086,26 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="23" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="24" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1071,47 +1114,9 @@
   <dxfs count="134">
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
         <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCDCD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE1E1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
       </font>
       <fill>
         <patternFill patternType="none">
@@ -1121,7 +1126,9 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FFC00000"/>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FF005C00"/>
       </font>
       <fill>
         <patternFill patternType="none">
@@ -1143,9 +1150,7 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color rgb="FF005C00"/>
+        <color rgb="FFC00000"/>
       </font>
       <fill>
         <patternFill patternType="none">
@@ -1167,9 +1172,7 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color auto="1"/>
+        <color rgb="FFC00000"/>
       </font>
       <fill>
         <patternFill patternType="none">
@@ -1183,6 +1186,26 @@
       </font>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFFE1E1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCDCD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
           <bgColor theme="9" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
@@ -1203,7 +1226,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFCDCD"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1213,13 +1236,15 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFE1E1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FF005C00"/>
       </font>
       <fill>
         <patternFill patternType="none">
@@ -1229,7 +1254,9 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FFC00000"/>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FF005C00"/>
       </font>
       <fill>
         <patternFill patternType="none">
@@ -1238,10 +1265,29 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCDEBFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
-        <color rgb="FF005C00"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF5F9FD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color auto="1"/>
       </font>
       <fill>
         <patternFill patternType="none">
@@ -1263,9 +1309,7 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color rgb="FF005C00"/>
+        <color rgb="FFC00000"/>
       </font>
       <fill>
         <patternFill patternType="none">
@@ -1275,9 +1319,7 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color auto="1"/>
+        <color rgb="FFC00000"/>
       </font>
       <fill>
         <patternFill patternType="none">
@@ -1287,6 +1329,203 @@
     </dxf>
     <dxf>
       <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFE1E1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCDCD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF006600"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF006600"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF0000FF"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF0000FF"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF0000FF"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF0000FF"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF0000FF"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF0000FF"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCDCD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCDEBFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <color auto="1"/>
@@ -1298,195 +1537,10 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCDEBFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF006600"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF006600"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
         <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF0000FF"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF0000FF"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF0000FF"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF0000FF"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF0000FF"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF0000FF"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCDCD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE1E1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
       </font>
       <fill>
         <patternFill patternType="none">
@@ -1496,7 +1550,9 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FFC00000"/>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FF005C00"/>
       </font>
       <fill>
         <patternFill patternType="none">
@@ -1530,9 +1586,7 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color rgb="FF005C00"/>
+        <color rgb="FFC00000"/>
       </font>
       <fill>
         <patternFill patternType="none">
@@ -1542,9 +1596,7 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color auto="1"/>
+        <color rgb="FFC00000"/>
       </font>
       <fill>
         <patternFill patternType="none">
@@ -1554,6 +1606,36 @@
     </dxf>
     <dxf>
       <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFE1E1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF008000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF008000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF0000FF"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <color auto="1"/>
@@ -1572,24 +1654,11 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF008000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF008000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF0000FF"/>
-      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCDEBFF"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -1604,55 +1673,10 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCDEBFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
         <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCDCD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE1E1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
       </font>
       <fill>
         <patternFill patternType="none">
@@ -1662,7 +1686,9 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FFC00000"/>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FF005C00"/>
       </font>
       <fill>
         <patternFill patternType="none">
@@ -1672,9 +1698,7 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color rgb="FF005C00"/>
+        <color rgb="FFC00000"/>
       </font>
       <fill>
         <patternFill patternType="none">
@@ -1684,6 +1708,26 @@
     </dxf>
     <dxf>
       <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <color rgb="FF005C00"/>
@@ -1696,9 +1740,7 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color rgb="FF005C00"/>
+        <color rgb="FFC00000"/>
       </font>
       <fill>
         <patternFill patternType="none">
@@ -1708,9 +1750,29 @@
     </dxf>
     <dxf>
       <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFE1E1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCDCD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
-        <color auto="1"/>
+        <color rgb="FF005C00"/>
       </font>
       <fill>
         <patternFill patternType="none">
@@ -1720,20 +1782,11 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
         <color auto="1"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFF5F9FD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCDEBFF"/>
+          <bgColor rgb="FFFFE1E1"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1743,37 +1796,27 @@
       </font>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFFCDCD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
           <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCDCD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE1E1"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1865,6 +1908,58 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor theme="0" tint="-0.24994659260841701"/>
@@ -1872,136 +1967,141 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF0000FF"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF0000FF"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF0000FF"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF0000FF"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF0000FF"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF0000FF"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF006600"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF006600"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFE5E5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD3E6F5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <color auto="1"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FF006600"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FF006600"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
         <color rgb="FFC00000"/>
       </font>
     </dxf>
     <dxf>
       <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF0000FF"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF0000FF"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF0000FF"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF0000FF"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF0000FF"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF0000FF"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
+        <b val="0"/>
+        <i val="0"/>
         <color rgb="FFC00000"/>
       </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF006600"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF006600"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE5E5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
       <fill>
         <patternFill>
           <bgColor theme="4" tint="0.59996337778862885"/>
@@ -2009,18 +2109,53 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD3E6F5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
         <color auto="1"/>
       </font>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFFD9D9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFE7E7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
           <bgColor theme="9" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
@@ -2029,156 +2164,36 @@
       <font>
         <b val="0"/>
         <i val="0"/>
-        <color rgb="FF006600"/>
+        <color rgb="FF005000"/>
       </font>
     </dxf>
     <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
-        <color rgb="FF006600"/>
-      </font>
+        <color rgb="FF005000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFD9D9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE7E7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color rgb="FF005000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color rgb="FF005000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCDCD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE1E1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
+        <color rgb="FF005C00"/>
       </font>
       <fill>
         <patternFill patternType="none">
@@ -2198,9 +2213,7 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color rgb="FF005C00"/>
+        <color rgb="FFC00000"/>
       </font>
       <fill>
         <patternFill patternType="none">
@@ -2210,9 +2223,39 @@
     </dxf>
     <dxf>
       <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFE1E1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCDCD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
-        <color rgb="FF005C00"/>
+        <color auto="1"/>
       </font>
       <fill>
         <patternFill patternType="none">
@@ -2236,7 +2279,7 @@
       <font>
         <b val="0"/>
         <i val="0"/>
-        <color auto="1"/>
+        <color rgb="FF005C00"/>
       </font>
       <fill>
         <patternFill patternType="none">
@@ -2574,192 +2617,192 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14D71DC9-2596-441F-B45A-63A457CE14D1}">
-  <dimension ref="A1:AI29"/>
+  <dimension ref="A1:AI27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="19.109375" customWidth="1"/>
-    <col min="3" max="3" width="17.6640625" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="32" t="s">
+    <row r="1" spans="1:35" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="77" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="38" t="s">
+      <c r="B1" s="78"/>
+      <c r="C1" s="78"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="78"/>
+      <c r="H1" s="79"/>
+      <c r="I1" s="66" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="38"/>
-      <c r="K1" s="38"/>
-      <c r="L1" s="38"/>
-      <c r="M1" s="38"/>
-      <c r="N1" s="38"/>
-      <c r="O1" s="39"/>
-      <c r="P1" s="39"/>
-      <c r="Q1" s="39"/>
-      <c r="R1" s="39"/>
-      <c r="S1" s="39"/>
-      <c r="T1" s="39"/>
-      <c r="U1" s="39"/>
-      <c r="V1" s="39"/>
-      <c r="W1" s="39"/>
-      <c r="X1" s="39"/>
-      <c r="Y1" s="39"/>
-      <c r="Z1" s="39"/>
-      <c r="AA1" s="40" t="s">
+      <c r="J1" s="66"/>
+      <c r="K1" s="66"/>
+      <c r="L1" s="66"/>
+      <c r="M1" s="66"/>
+      <c r="N1" s="66"/>
+      <c r="O1" s="65"/>
+      <c r="P1" s="65"/>
+      <c r="Q1" s="65"/>
+      <c r="R1" s="65"/>
+      <c r="S1" s="65"/>
+      <c r="T1" s="65"/>
+      <c r="U1" s="65"/>
+      <c r="V1" s="65"/>
+      <c r="W1" s="65"/>
+      <c r="X1" s="65"/>
+      <c r="Y1" s="65"/>
+      <c r="Z1" s="65"/>
+      <c r="AA1" s="83" t="s">
         <v>2</v>
       </c>
-      <c r="AB1" s="40"/>
-      <c r="AC1" s="40"/>
-      <c r="AD1" s="40"/>
-      <c r="AE1" s="40"/>
-      <c r="AF1" s="40"/>
-      <c r="AG1" s="40"/>
-      <c r="AH1" s="40"/>
-      <c r="AI1" s="40"/>
+      <c r="AB1" s="83"/>
+      <c r="AC1" s="83"/>
+      <c r="AD1" s="83"/>
+      <c r="AE1" s="83"/>
+      <c r="AF1" s="83"/>
+      <c r="AG1" s="83"/>
+      <c r="AH1" s="83"/>
+      <c r="AI1" s="83"/>
     </row>
-    <row r="2" spans="1:35" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="35"/>
-      <c r="B2" s="36"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="38" t="s">
+    <row r="2" spans="1:35" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="80"/>
+      <c r="B2" s="81"/>
+      <c r="C2" s="81"/>
+      <c r="D2" s="81"/>
+      <c r="E2" s="81"/>
+      <c r="F2" s="81"/>
+      <c r="G2" s="81"/>
+      <c r="H2" s="82"/>
+      <c r="I2" s="66" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="38"/>
-      <c r="K2" s="38"/>
-      <c r="L2" s="38"/>
-      <c r="M2" s="38"/>
-      <c r="N2" s="38"/>
-      <c r="O2" s="41"/>
-      <c r="P2" s="41"/>
-      <c r="Q2" s="41"/>
-      <c r="R2" s="41"/>
-      <c r="S2" s="41"/>
-      <c r="T2" s="41"/>
-      <c r="U2" s="41"/>
-      <c r="V2" s="41"/>
+      <c r="J2" s="66"/>
+      <c r="K2" s="66"/>
+      <c r="L2" s="66"/>
+      <c r="M2" s="66"/>
+      <c r="N2" s="66"/>
+      <c r="O2" s="63"/>
+      <c r="P2" s="63"/>
+      <c r="Q2" s="63"/>
+      <c r="R2" s="63"/>
+      <c r="S2" s="63"/>
+      <c r="T2" s="63"/>
+      <c r="U2" s="63"/>
+      <c r="V2" s="63"/>
       <c r="W2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="X2" s="42"/>
-      <c r="Y2" s="43"/>
-      <c r="Z2" s="43"/>
-      <c r="AA2" s="40"/>
-      <c r="AB2" s="40"/>
-      <c r="AC2" s="40"/>
-      <c r="AD2" s="40"/>
-      <c r="AE2" s="40"/>
-      <c r="AF2" s="40"/>
-      <c r="AG2" s="40"/>
-      <c r="AH2" s="40"/>
-      <c r="AI2" s="40"/>
+      <c r="X2" s="84"/>
+      <c r="Y2" s="85"/>
+      <c r="Z2" s="85"/>
+      <c r="AA2" s="83"/>
+      <c r="AB2" s="83"/>
+      <c r="AC2" s="83"/>
+      <c r="AD2" s="83"/>
+      <c r="AE2" s="83"/>
+      <c r="AF2" s="83"/>
+      <c r="AG2" s="83"/>
+      <c r="AH2" s="83"/>
+      <c r="AI2" s="83"/>
     </row>
-    <row r="3" spans="1:35" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="44" t="s">
+    <row r="3" spans="1:35" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="44"/>
-      <c r="C3" s="45"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="45"/>
-      <c r="G3" s="45"/>
-      <c r="H3" s="45"/>
-      <c r="I3" s="38" t="s">
+      <c r="B3" s="64"/>
+      <c r="C3" s="86"/>
+      <c r="D3" s="86"/>
+      <c r="E3" s="86"/>
+      <c r="F3" s="86"/>
+      <c r="G3" s="86"/>
+      <c r="H3" s="86"/>
+      <c r="I3" s="66" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="38"/>
-      <c r="K3" s="38"/>
-      <c r="L3" s="38"/>
-      <c r="M3" s="38"/>
-      <c r="N3" s="38"/>
-      <c r="O3" s="41"/>
-      <c r="P3" s="41"/>
-      <c r="Q3" s="41"/>
-      <c r="R3" s="41"/>
-      <c r="S3" s="41"/>
-      <c r="T3" s="41"/>
-      <c r="U3" s="41"/>
-      <c r="V3" s="41"/>
-      <c r="W3" s="41"/>
-      <c r="X3" s="41"/>
-      <c r="Y3" s="41"/>
-      <c r="Z3" s="41"/>
-      <c r="AA3" s="40"/>
-      <c r="AB3" s="40"/>
-      <c r="AC3" s="40"/>
-      <c r="AD3" s="40"/>
-      <c r="AE3" s="40"/>
-      <c r="AF3" s="40"/>
-      <c r="AG3" s="40"/>
-      <c r="AH3" s="40"/>
-      <c r="AI3" s="40"/>
+      <c r="J3" s="66"/>
+      <c r="K3" s="66"/>
+      <c r="L3" s="66"/>
+      <c r="M3" s="66"/>
+      <c r="N3" s="66"/>
+      <c r="O3" s="63"/>
+      <c r="P3" s="63"/>
+      <c r="Q3" s="63"/>
+      <c r="R3" s="63"/>
+      <c r="S3" s="63"/>
+      <c r="T3" s="63"/>
+      <c r="U3" s="63"/>
+      <c r="V3" s="63"/>
+      <c r="W3" s="63"/>
+      <c r="X3" s="63"/>
+      <c r="Y3" s="63"/>
+      <c r="Z3" s="63"/>
+      <c r="AA3" s="83"/>
+      <c r="AB3" s="83"/>
+      <c r="AC3" s="83"/>
+      <c r="AD3" s="83"/>
+      <c r="AE3" s="83"/>
+      <c r="AF3" s="83"/>
+      <c r="AG3" s="83"/>
+      <c r="AH3" s="83"/>
+      <c r="AI3" s="83"/>
     </row>
-    <row r="4" spans="1:35" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="44" t="s">
+    <row r="4" spans="1:35" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="64" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="44"/>
-      <c r="C4" s="39"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="39"/>
-      <c r="G4" s="39"/>
-      <c r="H4" s="39"/>
-      <c r="I4" s="38" t="s">
+      <c r="B4" s="64"/>
+      <c r="C4" s="65"/>
+      <c r="D4" s="65"/>
+      <c r="E4" s="65"/>
+      <c r="F4" s="65"/>
+      <c r="G4" s="65"/>
+      <c r="H4" s="65"/>
+      <c r="I4" s="66" t="s">
         <v>8</v>
       </c>
-      <c r="J4" s="38"/>
-      <c r="K4" s="38"/>
-      <c r="L4" s="38"/>
-      <c r="M4" s="38"/>
-      <c r="N4" s="38"/>
-      <c r="O4" s="68"/>
-      <c r="P4" s="69"/>
-      <c r="Q4" s="69"/>
-      <c r="R4" s="69"/>
-      <c r="S4" s="69"/>
-      <c r="T4" s="69"/>
-      <c r="U4" s="69"/>
-      <c r="V4" s="69"/>
-      <c r="W4" s="69"/>
-      <c r="X4" s="69"/>
-      <c r="Y4" s="69"/>
-      <c r="Z4" s="70"/>
-      <c r="AA4" s="40"/>
-      <c r="AB4" s="40"/>
-      <c r="AC4" s="40"/>
-      <c r="AD4" s="40"/>
-      <c r="AE4" s="40"/>
-      <c r="AF4" s="40"/>
-      <c r="AG4" s="40"/>
-      <c r="AH4" s="40"/>
-      <c r="AI4" s="40"/>
+      <c r="J4" s="66"/>
+      <c r="K4" s="66"/>
+      <c r="L4" s="66"/>
+      <c r="M4" s="66"/>
+      <c r="N4" s="66"/>
+      <c r="O4" s="74"/>
+      <c r="P4" s="75"/>
+      <c r="Q4" s="75"/>
+      <c r="R4" s="75"/>
+      <c r="S4" s="75"/>
+      <c r="T4" s="75"/>
+      <c r="U4" s="75"/>
+      <c r="V4" s="75"/>
+      <c r="W4" s="75"/>
+      <c r="X4" s="75"/>
+      <c r="Y4" s="75"/>
+      <c r="Z4" s="76"/>
+      <c r="AA4" s="83"/>
+      <c r="AB4" s="83"/>
+      <c r="AC4" s="83"/>
+      <c r="AD4" s="83"/>
+      <c r="AE4" s="83"/>
+      <c r="AF4" s="83"/>
+      <c r="AG4" s="83"/>
+      <c r="AH4" s="83"/>
+      <c r="AI4" s="83"/>
     </row>
-    <row r="5" spans="1:35" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:35" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="86" t="s">
+      <c r="B5" s="67" t="s">
         <v>77</v>
       </c>
-      <c r="C5" s="87"/>
+      <c r="C5" s="68"/>
       <c r="D5" s="27">
         <v>1</v>
       </c>
@@ -2857,14 +2900,14 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:35" ht="54" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="77">
+    <row r="6" spans="1:35" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="69">
         <v>1</v>
       </c>
-      <c r="B6" s="78" t="s">
+      <c r="B6" s="72" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="79"/>
+      <c r="C6" s="73"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
@@ -2897,12 +2940,12 @@
       <c r="AG6" s="23"/>
       <c r="AH6" s="23"/>
     </row>
-    <row r="7" spans="1:35" ht="45.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="80"/>
-      <c r="B7" s="78" t="s">
+    <row r="7" spans="1:35" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="70"/>
+      <c r="B7" s="72" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="79"/>
+      <c r="C7" s="73"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
@@ -2935,12 +2978,12 @@
       <c r="AG7" s="24"/>
       <c r="AH7" s="24"/>
     </row>
-    <row r="8" spans="1:35" ht="57.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="81"/>
-      <c r="B8" s="78" t="s">
+    <row r="8" spans="1:35" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="71"/>
+      <c r="B8" s="72" t="s">
         <v>73</v>
       </c>
-      <c r="C8" s="79"/>
+      <c r="C8" s="73"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
@@ -2977,14 +3020,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:35" ht="65.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:35" ht="65.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="18">
         <v>2</v>
       </c>
-      <c r="B9" s="46" t="s">
+      <c r="B9" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="47"/>
+      <c r="C9" s="46"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
@@ -3021,14 +3064,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:35" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="82">
+    <row r="10" spans="1:35" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="32">
         <v>3</v>
       </c>
-      <c r="B10" s="83" t="s">
+      <c r="B10" s="54" t="s">
         <v>74</v>
       </c>
-      <c r="C10" s="84"/>
+      <c r="C10" s="55"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
@@ -3065,14 +3108,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:35" ht="64.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:35" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="18">
         <v>4</v>
       </c>
-      <c r="B11" s="51" t="s">
+      <c r="B11" s="56" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="47"/>
+      <c r="C11" s="46"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
@@ -3105,11 +3148,11 @@
       <c r="AG11" s="25"/>
       <c r="AH11" s="25"/>
     </row>
-    <row r="12" spans="1:35" ht="51.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="48">
+    <row r="12" spans="1:35" ht="51.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="41">
         <v>5</v>
       </c>
-      <c r="B12" s="52" t="s">
+      <c r="B12" s="43" t="s">
         <v>17</v>
       </c>
       <c r="C12" s="22" t="s">
@@ -3147,9 +3190,9 @@
       <c r="AG12" s="24"/>
       <c r="AH12" s="24"/>
     </row>
-    <row r="13" spans="1:35" ht="45.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="49"/>
-      <c r="B13" s="53"/>
+    <row r="13" spans="1:35" ht="45.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="57"/>
+      <c r="B13" s="58"/>
       <c r="C13" s="21" t="s">
         <v>19</v>
       </c>
@@ -3185,9 +3228,9 @@
       <c r="AG13" s="24"/>
       <c r="AH13" s="24"/>
     </row>
-    <row r="14" spans="1:35" ht="41.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="49"/>
-      <c r="B14" s="53"/>
+    <row r="14" spans="1:35" ht="41.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="57"/>
+      <c r="B14" s="58"/>
       <c r="C14" s="21" t="s">
         <v>20</v>
       </c>
@@ -3227,9 +3270,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:35" ht="56.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="50"/>
-      <c r="B15" s="54"/>
+    <row r="15" spans="1:35" ht="56.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="42"/>
+      <c r="B15" s="44"/>
       <c r="C15" s="21" t="s">
         <v>21</v>
       </c>
@@ -3265,11 +3308,11 @@
       <c r="AG15" s="25"/>
       <c r="AH15" s="25"/>
     </row>
-    <row r="16" spans="1:35" ht="54" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="55">
+    <row r="16" spans="1:35" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="59">
         <v>6</v>
       </c>
-      <c r="B16" s="57" t="s">
+      <c r="B16" s="61" t="s">
         <v>22</v>
       </c>
       <c r="C16" s="19" t="s">
@@ -3307,9 +3350,9 @@
       <c r="AG16" s="25"/>
       <c r="AH16" s="25"/>
     </row>
-    <row r="17" spans="1:35" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="56"/>
-      <c r="B17" s="58"/>
+    <row r="17" spans="1:35" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="60"/>
+      <c r="B17" s="62"/>
       <c r="C17" s="20" t="s">
         <v>24</v>
       </c>
@@ -3349,11 +3392,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:35" ht="42" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="48">
+    <row r="18" spans="1:35" ht="42" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="41">
         <v>7</v>
       </c>
-      <c r="B18" s="52" t="s">
+      <c r="B18" s="43" t="s">
         <v>25</v>
       </c>
       <c r="C18" s="21" t="s">
@@ -3391,9 +3434,9 @@
       <c r="AG18" s="25"/>
       <c r="AH18" s="25"/>
     </row>
-    <row r="19" spans="1:35" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="50"/>
-      <c r="B19" s="54"/>
+    <row r="19" spans="1:35" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="42"/>
+      <c r="B19" s="44"/>
       <c r="C19" s="21" t="s">
         <v>24</v>
       </c>
@@ -3433,14 +3476,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:35" ht="73.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:35" ht="73.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="18">
         <v>8</v>
       </c>
-      <c r="B20" s="46" t="s">
+      <c r="B20" s="45" t="s">
         <v>26</v>
       </c>
-      <c r="C20" s="47"/>
+      <c r="C20" s="46"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
@@ -3477,7 +3520,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:35" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
       <c r="B21" s="8"/>
       <c r="C21" s="7"/>
@@ -3514,46 +3557,46 @@
       <c r="AH21" s="7"/>
       <c r="AI21" s="9"/>
     </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:35" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
       <c r="B22" s="8"/>
       <c r="C22" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D22" s="61"/>
-      <c r="E22" s="62"/>
-      <c r="F22" s="62"/>
-      <c r="G22" s="62"/>
-      <c r="H22" s="62"/>
-      <c r="I22" s="62"/>
-      <c r="J22" s="62"/>
-      <c r="K22" s="62"/>
-      <c r="L22" s="62"/>
-      <c r="M22" s="62"/>
-      <c r="N22" s="62"/>
-      <c r="O22" s="62"/>
-      <c r="P22" s="62"/>
-      <c r="Q22" s="62"/>
-      <c r="R22" s="62"/>
-      <c r="S22" s="62"/>
-      <c r="T22" s="62"/>
-      <c r="U22" s="62"/>
-      <c r="V22" s="62"/>
-      <c r="W22" s="62"/>
-      <c r="X22" s="62"/>
-      <c r="Y22" s="62"/>
-      <c r="Z22" s="62"/>
-      <c r="AA22" s="62"/>
-      <c r="AB22" s="62"/>
-      <c r="AC22" s="62"/>
-      <c r="AD22" s="62"/>
-      <c r="AE22" s="62"/>
-      <c r="AF22" s="62"/>
-      <c r="AG22" s="62"/>
-      <c r="AH22" s="62"/>
-      <c r="AI22" s="63"/>
+      <c r="D22" s="47"/>
+      <c r="E22" s="48"/>
+      <c r="F22" s="48"/>
+      <c r="G22" s="48"/>
+      <c r="H22" s="48"/>
+      <c r="I22" s="48"/>
+      <c r="J22" s="48"/>
+      <c r="K22" s="48"/>
+      <c r="L22" s="48"/>
+      <c r="M22" s="48"/>
+      <c r="N22" s="48"/>
+      <c r="O22" s="48"/>
+      <c r="P22" s="48"/>
+      <c r="Q22" s="48"/>
+      <c r="R22" s="48"/>
+      <c r="S22" s="48"/>
+      <c r="T22" s="48"/>
+      <c r="U22" s="48"/>
+      <c r="V22" s="48"/>
+      <c r="W22" s="48"/>
+      <c r="X22" s="48"/>
+      <c r="Y22" s="48"/>
+      <c r="Z22" s="48"/>
+      <c r="AA22" s="48"/>
+      <c r="AB22" s="48"/>
+      <c r="AC22" s="48"/>
+      <c r="AD22" s="48"/>
+      <c r="AE22" s="48"/>
+      <c r="AF22" s="48"/>
+      <c r="AG22" s="48"/>
+      <c r="AH22" s="48"/>
+      <c r="AI22" s="49"/>
     </row>
-    <row r="23" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A23" s="9"/>
       <c r="B23" s="11"/>
       <c r="C23" s="12"/>
@@ -3590,7 +3633,7 @@
       <c r="AH23" s="9"/>
       <c r="AI23" s="9"/>
     </row>
-    <row r="24" spans="1:35" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:35" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="9"/>
       <c r="B24" s="11"/>
       <c r="C24" s="10" t="s">
@@ -3599,31 +3642,31 @@
       <c r="D24" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="E24" s="64" t="s">
+      <c r="E24" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="F24" s="64"/>
-      <c r="G24" s="65"/>
+      <c r="F24" s="50"/>
+      <c r="G24" s="51"/>
       <c r="H24" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="I24" s="66" t="s">
+      <c r="I24" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="J24" s="66"/>
-      <c r="K24" s="66"/>
-      <c r="L24" s="66"/>
-      <c r="M24" s="66"/>
-      <c r="N24" s="66"/>
-      <c r="O24" s="67"/>
+      <c r="J24" s="52"/>
+      <c r="K24" s="52"/>
+      <c r="L24" s="52"/>
+      <c r="M24" s="52"/>
+      <c r="N24" s="52"/>
+      <c r="O24" s="53"/>
       <c r="P24" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="Q24" s="64" t="s">
+      <c r="Q24" s="50" t="s">
         <v>32</v>
       </c>
-      <c r="R24" s="64"/>
-      <c r="S24" s="65"/>
+      <c r="R24" s="50"/>
+      <c r="S24" s="51"/>
       <c r="T24" s="9"/>
       <c r="U24" s="9"/>
       <c r="V24" s="9"/>
@@ -3641,192 +3684,198 @@
       <c r="AH24" s="9"/>
       <c r="AI24" s="9"/>
     </row>
-    <row r="25" spans="1:35" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:35" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="9"/>
-      <c r="B25" s="11"/>
+      <c r="B25" s="87" t="s">
+        <v>78</v>
+      </c>
       <c r="C25" s="11"/>
       <c r="D25" s="30" t="s">
         <v>75</v>
       </c>
-      <c r="E25" s="73" t="s">
+      <c r="E25" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="F25" s="73"/>
-      <c r="G25" s="74"/>
+      <c r="F25" s="33"/>
+      <c r="G25" s="36"/>
       <c r="H25" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="I25" s="75" t="s">
+      <c r="I25" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="J25" s="75"/>
-      <c r="K25" s="76"/>
+      <c r="J25" s="37"/>
+      <c r="K25" s="38"/>
       <c r="L25" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="M25" s="59" t="s">
+      <c r="M25" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="N25" s="59"/>
-      <c r="O25" s="60"/>
+      <c r="N25" s="34"/>
+      <c r="O25" s="35"/>
       <c r="P25" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="Q25" s="59" t="s">
+      <c r="Q25" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="R25" s="59"/>
-      <c r="S25" s="60"/>
+      <c r="R25" s="34"/>
+      <c r="S25" s="35"/>
       <c r="T25" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="U25" s="59" t="s">
+      <c r="U25" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="V25" s="59"/>
-      <c r="W25" s="60"/>
+      <c r="V25" s="34"/>
+      <c r="W25" s="35"/>
       <c r="X25" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="Y25" s="59" t="s">
+      <c r="Y25" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="Z25" s="59"/>
-      <c r="AA25" s="60"/>
+      <c r="Z25" s="34"/>
+      <c r="AA25" s="35"/>
       <c r="AB25" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="AC25" s="59" t="s">
+      <c r="AC25" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="AD25" s="59"/>
-      <c r="AE25" s="60"/>
+      <c r="AD25" s="34"/>
+      <c r="AE25" s="35"/>
       <c r="AF25" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="AG25" s="59" t="s">
+      <c r="AG25" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="AH25" s="59"/>
-      <c r="AI25" s="60"/>
+      <c r="AH25" s="34"/>
+      <c r="AI25" s="35"/>
     </row>
-    <row r="26" spans="1:35" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:35" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="9"/>
-      <c r="B26" s="11"/>
+      <c r="B26" s="88" t="s">
+        <v>79</v>
+      </c>
       <c r="C26" s="11"/>
       <c r="D26" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="E26" s="59" t="s">
+      <c r="E26" s="34" t="s">
         <v>48</v>
       </c>
-      <c r="F26" s="59"/>
-      <c r="G26" s="60"/>
+      <c r="F26" s="34"/>
+      <c r="G26" s="35"/>
       <c r="H26" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="I26" s="71" t="s">
+      <c r="I26" s="39" t="s">
         <v>50</v>
       </c>
-      <c r="J26" s="71"/>
-      <c r="K26" s="72"/>
+      <c r="J26" s="39"/>
+      <c r="K26" s="40"/>
       <c r="L26" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="M26" s="59" t="s">
+      <c r="M26" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="N26" s="59"/>
-      <c r="O26" s="60"/>
+      <c r="N26" s="34"/>
+      <c r="O26" s="35"/>
       <c r="P26" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="Q26" s="59" t="s">
+      <c r="Q26" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="R26" s="59"/>
-      <c r="S26" s="60"/>
+      <c r="R26" s="34"/>
+      <c r="S26" s="35"/>
       <c r="T26" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="U26" s="59" t="s">
+      <c r="U26" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="V26" s="59"/>
-      <c r="W26" s="60"/>
+      <c r="V26" s="34"/>
+      <c r="W26" s="35"/>
       <c r="X26" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="Y26" s="59" t="s">
+      <c r="Y26" s="34" t="s">
         <v>58</v>
       </c>
-      <c r="Z26" s="59"/>
-      <c r="AA26" s="60"/>
+      <c r="Z26" s="34"/>
+      <c r="AA26" s="35"/>
       <c r="AB26" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="AC26" s="73" t="s">
+      <c r="AC26" s="33" t="s">
         <v>60</v>
       </c>
-      <c r="AD26" s="73"/>
-      <c r="AE26" s="74"/>
+      <c r="AD26" s="33"/>
+      <c r="AE26" s="36"/>
       <c r="AF26" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="AG26" s="73" t="s">
+      <c r="AG26" s="33" t="s">
         <v>62</v>
       </c>
-      <c r="AH26" s="73"/>
-      <c r="AI26" s="74"/>
+      <c r="AH26" s="33"/>
+      <c r="AI26" s="36"/>
     </row>
-    <row r="27" spans="1:35" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:35" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="9"/>
-      <c r="B27" s="11"/>
+      <c r="B27" s="89" t="s">
+        <v>80</v>
+      </c>
       <c r="C27" s="11"/>
       <c r="D27" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="E27" s="73" t="s">
+      <c r="E27" s="33" t="s">
         <v>64</v>
       </c>
-      <c r="F27" s="73"/>
-      <c r="G27" s="73"/>
+      <c r="F27" s="33"/>
+      <c r="G27" s="33"/>
       <c r="H27" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="I27" s="59" t="s">
+      <c r="I27" s="34" t="s">
         <v>66</v>
       </c>
-      <c r="J27" s="59"/>
-      <c r="K27" s="59"/>
-      <c r="L27" s="59"/>
-      <c r="M27" s="59"/>
-      <c r="N27" s="59"/>
-      <c r="O27" s="60"/>
+      <c r="J27" s="34"/>
+      <c r="K27" s="34"/>
+      <c r="L27" s="34"/>
+      <c r="M27" s="34"/>
+      <c r="N27" s="34"/>
+      <c r="O27" s="35"/>
       <c r="P27" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="Q27" s="73" t="s">
+      <c r="Q27" s="33" t="s">
         <v>68</v>
       </c>
-      <c r="R27" s="73"/>
-      <c r="S27" s="74"/>
+      <c r="R27" s="33"/>
+      <c r="S27" s="36"/>
       <c r="T27" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="U27" s="73" t="s">
+      <c r="U27" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="V27" s="73"/>
-      <c r="W27" s="74"/>
+      <c r="V27" s="33"/>
+      <c r="W27" s="36"/>
       <c r="X27" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="Y27" s="73" t="s">
+      <c r="Y27" s="33" t="s">
         <v>72</v>
       </c>
-      <c r="Z27" s="73"/>
-      <c r="AA27" s="74"/>
+      <c r="Z27" s="33"/>
+      <c r="AA27" s="36"/>
       <c r="AB27" s="9"/>
       <c r="AC27" s="9"/>
       <c r="AD27" s="9"/>
@@ -3836,17 +3885,42 @@
       <c r="AH27" s="9"/>
       <c r="AI27" s="9"/>
     </row>
-    <row r="29" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="D29" s="85"/>
-      <c r="E29" s="85"/>
-    </row>
   </sheetData>
   <mergeCells count="55">
-    <mergeCell ref="E27:G27"/>
-    <mergeCell ref="I27:O27"/>
-    <mergeCell ref="Q27:S27"/>
-    <mergeCell ref="U27:W27"/>
-    <mergeCell ref="Y27:AA27"/>
+    <mergeCell ref="A1:H2"/>
+    <mergeCell ref="I1:N1"/>
+    <mergeCell ref="O1:Z1"/>
+    <mergeCell ref="AA1:AI4"/>
+    <mergeCell ref="I2:N2"/>
+    <mergeCell ref="O2:V2"/>
+    <mergeCell ref="X2:Z2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:H3"/>
+    <mergeCell ref="I3:N3"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="O3:Z3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:H4"/>
+    <mergeCell ref="I4:N4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="O4:Z4"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="B12:B15"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="D22:AI22"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="I24:O24"/>
+    <mergeCell ref="Q24:S24"/>
     <mergeCell ref="Y26:AA26"/>
     <mergeCell ref="AC26:AE26"/>
     <mergeCell ref="AG26:AI26"/>
@@ -3861,70 +3935,41 @@
     <mergeCell ref="Q26:S26"/>
     <mergeCell ref="U26:W26"/>
     <mergeCell ref="Y25:AA25"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="D22:AI22"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="I24:O24"/>
-    <mergeCell ref="Q24:S24"/>
     <mergeCell ref="AC25:AE25"/>
     <mergeCell ref="AG25:AI25"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="A12:A15"/>
-    <mergeCell ref="B12:B15"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="O3:Z3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:H4"/>
-    <mergeCell ref="I4:N4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="O4:Z4"/>
-    <mergeCell ref="A1:H2"/>
-    <mergeCell ref="I1:N1"/>
-    <mergeCell ref="O1:Z1"/>
-    <mergeCell ref="AA1:AI4"/>
-    <mergeCell ref="I2:N2"/>
-    <mergeCell ref="O2:V2"/>
-    <mergeCell ref="X2:Z2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:H3"/>
-    <mergeCell ref="I3:N3"/>
+    <mergeCell ref="E27:G27"/>
+    <mergeCell ref="I27:O27"/>
+    <mergeCell ref="Q27:S27"/>
+    <mergeCell ref="U27:W27"/>
+    <mergeCell ref="Y27:AA27"/>
   </mergeCells>
   <conditionalFormatting sqref="A1 I1:I4 O1:O4 A3:A4 C3:C4 D23:M23 X25:Y25 D26:D27 T26:Y27">
-    <cfRule type="cellIs" dxfId="133" priority="112" operator="equal">
-      <formula>"ŚWREH"</formula>
+    <cfRule type="cellIs" dxfId="133" priority="114" operator="equal">
+      <formula>"ZWO"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="132" priority="113" operator="equal">
       <formula>"ŚWREH"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="131" priority="114" operator="equal">
-      <formula>"ZWO"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="130" priority="115" operator="equal">
+    <cfRule type="cellIs" dxfId="131" priority="112" operator="equal">
+      <formula>"ŚWREH"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="130" priority="120" operator="equal">
+      <formula>"WD"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="129" priority="119" operator="equal">
+      <formula>"WN"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="128" priority="118" operator="equal">
+      <formula>"WN"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="127" priority="117" operator="equal">
+      <formula>"UW"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="126" priority="116" operator="equal">
+      <formula>"UWŻ"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="125" priority="115" operator="equal">
       <formula>"ZWL"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="129" priority="116" operator="equal">
-      <formula>"UWŻ"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="128" priority="117" operator="equal">
-      <formula>"UW"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="127" priority="118" operator="equal">
-      <formula>"WN"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="126" priority="119" operator="equal">
-      <formula>"WN"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="125" priority="120" operator="equal">
-      <formula>"WD"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1 I1:I4 O1:O4 A3:A4 C3:C4 D23:M23 X25:Y25 T26:Y27">
@@ -3933,29 +3978,29 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1 I1:I4 O1:O4 W2:X2 A3:A4 C3:C4">
-    <cfRule type="cellIs" dxfId="123" priority="105" operator="equal">
+    <cfRule type="cellIs" dxfId="123" priority="106" operator="equal">
+      <formula>"UW"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="122" priority="107" operator="equal">
+      <formula>"ZWO"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="121" priority="108" operator="equal">
+      <formula>"ZWL"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="120" priority="109" operator="equal">
+      <formula>"WŚ"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="119" priority="110" operator="equal">
+      <formula>"WD"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="118" priority="105" operator="equal">
       <formula>"UWŻ"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="122" priority="106" operator="equal">
-      <formula>"UW"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="121" priority="107" operator="equal">
-      <formula>"ZWO"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="120" priority="108" operator="equal">
-      <formula>"ZWL"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="119" priority="109" operator="equal">
-      <formula>"WŚ"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="118" priority="110" operator="equal">
-      <formula>"WD"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="117" priority="111" operator="equal">
       <formula>"WN"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:AI3 A4:O4 AA4:AI4 A5:AI5 A6:AH7 A8:AI10 A11:AH13 A14:AI14 A15:AH16 A17:AI17 A18:AH18 A19:AI23 A24:C25 T24:AI27 A26:D27">
+  <conditionalFormatting sqref="A1:AI3 A4:O4 AA4:AI4 A5:AI5 A6:AH7 A8:AI10 A11:AH13 A14:AI14 A15:AH16 A17:AI17 A18:AH18 A19:AI23 A24:C24 T24:AI27 C26:D27 A25:A27 C25">
     <cfRule type="cellIs" dxfId="116" priority="2" operator="equal">
       <formula>"WN"</formula>
     </cfRule>
@@ -3999,65 +4044,65 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10">
-    <cfRule type="cellIs" dxfId="103" priority="83" operator="equal">
-      <formula>"WN"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="102" priority="84" operator="equal">
-      <formula>"ZW"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="101" priority="85" operator="equal">
-      <formula>"DEL"</formula>
+    <cfRule type="cellIs" priority="90" operator="equal">
+      <formula>"WP"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="103" priority="89" operator="equal">
+      <formula>"D"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="102" priority="88" operator="equal">
+      <formula>"NP"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="101" priority="87" operator="equal">
+      <formula>"NB"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="100" priority="86" operator="equal">
       <formula>"NN"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="99" priority="87" operator="equal">
-      <formula>"NB"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="98" priority="88" operator="equal">
-      <formula>"NP"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="97" priority="89" operator="equal">
-      <formula>"D"</formula>
-    </cfRule>
-    <cfRule type="cellIs" priority="90" operator="equal">
-      <formula>"WP"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="96" priority="91" operator="equal">
-      <formula>"UB"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="95" priority="92" operator="equal">
-      <formula>"Uwych"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="94" priority="93" operator="equal">
-      <formula>"UR"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="93" priority="94" operator="equal">
-      <formula>"UM"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="92" priority="95" operator="equal">
-      <formula>"UOP"</formula>
+    <cfRule type="cellIs" dxfId="99" priority="85" operator="equal">
+      <formula>"DEL"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="98" priority="84" operator="equal">
+      <formula>"ZW"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="97" priority="83" operator="equal">
+      <formula>"WN"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="96" priority="102" operator="equal">
+      <formula>"W5"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="95" priority="104" operator="equal">
+      <formula>"WN"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="94" priority="103" operator="equal">
+      <formula>"WŚ"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="93" priority="99" operator="equal">
+      <formula>"UW"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="92" priority="97" operator="equal">
+      <formula>"UO"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="91" priority="98" operator="equal">
+      <formula>"UW"</formula>
     </cfRule>
     <cfRule type="cellIs" priority="96" operator="equal">
       <formula>"UO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="91" priority="97" operator="equal">
-      <formula>"UO"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="90" priority="98" operator="equal">
-      <formula>"UW"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="89" priority="99" operator="equal">
-      <formula>"UW"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="88" priority="102" operator="equal">
-      <formula>"W5"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="87" priority="103" operator="equal">
-      <formula>"WŚ"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="86" priority="104" operator="equal">
-      <formula>"WN"</formula>
+    <cfRule type="cellIs" dxfId="90" priority="95" operator="equal">
+      <formula>"UOP"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="89" priority="94" operator="equal">
+      <formula>"UM"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="88" priority="93" operator="equal">
+      <formula>"UR"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="87" priority="92" operator="equal">
+      <formula>"Uwych"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="86" priority="91" operator="equal">
+      <formula>"UB"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22">
@@ -4085,55 +4130,55 @@
     <cfRule type="cellIs" dxfId="78" priority="20" operator="equal">
       <formula>"UW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="77" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="24" operator="equal">
+      <formula>"WŚ"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="76" priority="23" operator="equal">
+      <formula>"WD"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="75" priority="22" operator="equal">
       <formula>"WN"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="76" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="21" operator="equal">
       <formula>"WN"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="75" priority="23" operator="equal">
-      <formula>"WD"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="74" priority="24" operator="equal">
-      <formula>"WŚ"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24">
-    <cfRule type="cellIs" dxfId="73" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="28" operator="equal">
+      <formula>"ŚWREH"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="72" priority="34" operator="equal">
+      <formula>"WN"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="71" priority="33" operator="equal">
+      <formula>"WN"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="70" priority="32" operator="equal">
+      <formula>"UW"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="69" priority="30" operator="equal">
+      <formula>"ZWL"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="68" priority="36" operator="equal">
+      <formula>"WŚ"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="67" priority="35" operator="equal">
       <formula>"WD"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="72" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="31" operator="equal">
+      <formula>"UWŻ"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="65" priority="29" operator="equal">
+      <formula>"ZWO"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="64" priority="27" operator="equal">
+      <formula>"ŚWREH"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="63" priority="26" operator="equal">
       <formula>"WD"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="71" priority="27" operator="equal">
-      <formula>"ŚWREH"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="70" priority="28" operator="equal">
-      <formula>"ŚWREH"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="69" priority="29" operator="equal">
-      <formula>"ZWO"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="30" operator="equal">
-      <formula>"ZWL"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="67" priority="31" operator="equal">
-      <formula>"UWŻ"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="32" operator="equal">
-      <formula>"UW"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="65" priority="33" operator="equal">
-      <formula>"WN"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="34" operator="equal">
-      <formula>"WN"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="63" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="25" operator="equal">
       <formula>"WD"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="36" operator="equal">
-      <formula>"WŚ"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D23:M23 X25:Y25 AF25:AG26 D26:D27 T26:Y27">
@@ -4150,52 +4195,52 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E18:G18 J18:AH18">
-    <cfRule type="cellIs" dxfId="58" priority="147" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="149" operator="equal">
+      <formula>"UW"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="57" priority="147" operator="equal">
       <formula>"OP"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="148" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="148" operator="equal">
       <formula>"CH"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="149" operator="equal">
-      <formula>"UW"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T25:U25">
-    <cfRule type="cellIs" dxfId="55" priority="37" operator="equal">
-      <formula>"WD"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="38" operator="equal">
-      <formula>"WD"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="53" priority="39" operator="equal">
-      <formula>"ŚWREH"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="40" operator="equal">
-      <formula>"ŚWREH"</formula>
+    <cfRule type="cellIs" dxfId="55" priority="45" operator="equal">
+      <formula>"WN"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="54" priority="44" operator="equal">
+      <formula>"UW"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="53" priority="43" operator="equal">
+      <formula>"UWŻ"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="52" priority="42" operator="equal">
+      <formula>"ZWL"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="51" priority="41" operator="equal">
       <formula>"ZWO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="42" operator="equal">
-      <formula>"ZWL"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="43" operator="equal">
-      <formula>"UWŻ"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="44" operator="equal">
-      <formula>"UW"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="45" operator="equal">
-      <formula>"WN"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="46" operator="equal">
-      <formula>"WN"</formula>
+    <cfRule type="cellIs" dxfId="50" priority="40" operator="equal">
+      <formula>"ŚWREH"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="49" priority="39" operator="equal">
+      <formula>"ŚWREH"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="48" priority="38" operator="equal">
+      <formula>"WD"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="47" priority="37" operator="equal">
+      <formula>"WD"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="46" priority="48" operator="equal">
+      <formula>"WŚ"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="45" priority="47" operator="equal">
       <formula>"WD"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="48" operator="equal">
-      <formula>"WŚ"</formula>
+    <cfRule type="cellIs" dxfId="44" priority="46" operator="equal">
+      <formula>"WN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W2">
@@ -4206,69 +4251,69 @@
       <formula>"WŚ"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA1 A5:AI5 A6:B6 D6:AH7 B7:B8 D8:AI10 A9:B9 A11:C12 D11:AH13 A13:A15 C13:C15 D14:AI14 D15:AH16 A16:C16 A17 C17:AI17 A18:AH18 A19 C19 D19:AI20 A20:B20 A21:AI21 A22:B22 D22 A23:C23 N23:AI23 A24:B24 T24:AI24 A25:C27 AB27:AH27">
-    <cfRule type="cellIs" dxfId="41" priority="124" operator="equal">
-      <formula>"WN"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="125" operator="equal">
-      <formula>"ZW"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="126" operator="equal">
-      <formula>"DEL"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="127" operator="equal">
-      <formula>"NN"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="128" operator="equal">
-      <formula>"NB"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="129" operator="equal">
+  <conditionalFormatting sqref="AA1 A5:AI5 A6:B6 D6:AH7 B7:B8 D8:AI10 A9:B9 A11:C12 D11:AH13 A13:A15 C13:C15 D14:AI14 D15:AH16 A16:C16 A17 C17:AI17 A18:AH18 A19 C19 D19:AI20 A20:B20 A21:AI21 A22:B22 D22 A23:C23 N23:AI23 A24:B24 T24:AI24 A25:A27 AB27:AH27 C25:C27">
+    <cfRule type="cellIs" dxfId="41" priority="129" operator="equal">
       <formula>"NP"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="130" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="130" operator="equal">
       <formula>"D"</formula>
     </cfRule>
     <cfRule type="cellIs" priority="131" operator="equal">
       <formula>"WP"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="132" operator="equal">
-      <formula>"UB"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="133" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="133" operator="equal">
       <formula>"Uwych"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="134" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="134" operator="equal">
       <formula>"UR"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="135" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="135" operator="equal">
       <formula>"UM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="136" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="128" operator="equal">
+      <formula>"NB"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="35" priority="136" operator="equal">
       <formula>"UOP"</formula>
     </cfRule>
     <cfRule type="cellIs" priority="137" operator="equal">
       <formula>"UO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="138" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="138" operator="equal">
       <formula>"UO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="139" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="139" operator="equal">
       <formula>"UW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="140" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="140" operator="equal">
       <formula>"UW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="143" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="143" operator="equal">
       <formula>"W5"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="144" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="144" operator="equal">
       <formula>"WŚ"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="145" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="145" operator="equal">
       <formula>"WN"</formula>
     </cfRule>
+    <cfRule type="cellIs" dxfId="28" priority="132" operator="equal">
+      <formula>"UB"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="27" priority="124" operator="equal">
+      <formula>"WN"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="26" priority="125" operator="equal">
+      <formula>"ZW"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="25" priority="126" operator="equal">
+      <formula>"DEL"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="127" operator="equal">
+      <formula>"NN"</formula>
+    </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA1 B5:AI5 D6:AH7 D8:AI10 B11:C12 D11:AH13 C13:C15 D14:AI14 D15:AH16 B16:C16 C17:AI17 B18:AH18 C19 D19:AI20 B20 B21:AI21 B22 D22 B23:C23 N23:AI23 B24 T24:AI24 B25:C27 AB27:AH27">
+  <conditionalFormatting sqref="AA1 B5:AI5 D6:AH7 D8:AI10 B11:C12 D11:AH13 C13:C15 D14:AI14 D15:AH16 B16:C16 C17:AI17 B18:AH18 C19 D19:AI20 B20 B21:AI21 B22 D22 B23:C23 N23:AI23 B24 T24:AI24 C25:C27 AB27:AH27">
     <cfRule type="cellIs" dxfId="23" priority="141" operator="equal">
       <formula>"OP"</formula>
     </cfRule>
@@ -4277,35 +4322,35 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB25:AC26">
-    <cfRule type="cellIs" dxfId="21" priority="49" operator="equal">
-      <formula>"WD"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="50" operator="equal">
-      <formula>"WD"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="51" operator="equal">
-      <formula>"ŚWREH"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="52" operator="equal">
-      <formula>"ŚWREH"</formula>
+    <cfRule type="cellIs" dxfId="21" priority="58" operator="equal">
+      <formula>"WN"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="20" priority="57" operator="equal">
+      <formula>"WN"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="19" priority="56" operator="equal">
+      <formula>"UW"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="55" operator="equal">
+      <formula>"UWŻ"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="17" priority="53" operator="equal">
       <formula>"ZWO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="51" operator="equal">
+      <formula>"ŚWREH"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="15" priority="50" operator="equal">
+      <formula>"WD"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="49" operator="equal">
+      <formula>"WD"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="13" priority="52" operator="equal">
+      <formula>"ŚWREH"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="54" operator="equal">
       <formula>"ZWL"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="55" operator="equal">
-      <formula>"UWŻ"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="56" operator="equal">
-      <formula>"UW"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="57" operator="equal">
-      <formula>"WN"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="58" operator="equal">
-      <formula>"WN"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="11" priority="59" operator="equal">
       <formula>"WD"</formula>
@@ -4315,35 +4360,35 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF25:AG26">
-    <cfRule type="cellIs" dxfId="9" priority="63" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="71" operator="equal">
+      <formula>"WD"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="72" operator="equal">
+      <formula>"WŚ"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="70" operator="equal">
+      <formula>"WN"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="69" operator="equal">
+      <formula>"WN"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="68" operator="equal">
+      <formula>"UW"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="66" operator="equal">
+      <formula>"ZWL"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="67" operator="equal">
+      <formula>"UWŻ"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="65" operator="equal">
+      <formula>"ZWO"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="64" operator="equal">
       <formula>"ŚWREH"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="64" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="63" operator="equal">
       <formula>"ŚWREH"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="65" operator="equal">
-      <formula>"ZWO"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="66" operator="equal">
-      <formula>"ZWL"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="67" operator="equal">
-      <formula>"UWŻ"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="68" operator="equal">
-      <formula>"UW"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="69" operator="equal">
-      <formula>"WN"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="70" operator="equal">
-      <formula>"WN"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="71" operator="equal">
-      <formula>"WD"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="72" operator="equal">
-      <formula>"WŚ"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4361,6 +4406,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100EFDF2CCD7F2A9549A796EF6A53171BC0" ma:contentTypeVersion="3" ma:contentTypeDescription="Utwórz nowy dokument." ma:contentTypeScope="" ma:versionID="17fdab98003bcb8b0eb99cbacf57169e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c61e7320-65a9-489d-8fd8-fad1618a30c1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fb41fdb58a90dd9e596254dbf35bfdcc" ns2:_="">
     <xsd:import namespace="c61e7320-65a9-489d-8fd8-fad1618a30c1"/>
@@ -4498,12 +4549,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4CD4CF01-6166-4398-8732-9E722BD8F723}">
   <ds:schemaRefs>
@@ -4513,6 +4558,15 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6DCF13F3-6C9E-4B19-BFCD-414BC58C8417}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5B9BB2D-0FA0-4FA8-93A3-294DB42DB928}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4528,13 +4582,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6DCF13F3-6C9E-4B19-BFCD-414BC58C8417}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>